<commit_message>
RTTBC24 Awesome Again Name Change to California Crown
</commit_message>
<xml_diff>
--- a/pdf/RTTBC24-Schedule-by-Division.xlsx
+++ b/pdf/RTTBC24-Schedule-by-Division.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/299f8723705ec823/Webmaster/gallop-racing.com/pdf/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1109" documentId="8_{DAECCBE5-FF72-4188-B2F1-1541968A3FDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D66DAF46-7088-45AF-B89E-19AA2886D818}"/>
+  <xr:revisionPtr revIDLastSave="1110" documentId="8_{DAECCBE5-FF72-4188-B2F1-1541968A3FDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6AA315F5-C56D-4CFD-A641-B8E10CBFF0D2}"/>
   <bookViews>
-    <workbookView xWindow="10545" yWindow="660" windowWidth="26955" windowHeight="20145" xr2:uid="{EAD27B02-19FE-4D48-9014-ED6E24DB84F0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{EAD27B02-19FE-4D48-9014-ED6E24DB84F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -296,9 +296,6 @@
     <t>Tokyo City Cup-G3</t>
   </si>
   <si>
-    <t>Awesome Again S.-G1</t>
-  </si>
-  <si>
     <t>Darley Alcibiades S.-G1</t>
   </si>
   <si>
@@ -384,6 +381,9 @@
   </si>
   <si>
     <t>Perryville S.-G3</t>
+  </si>
+  <si>
+    <t>California Crown S.-G1</t>
   </si>
 </sst>
 </file>
@@ -774,10 +774,100 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -786,15 +876,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -810,9 +891,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -833,84 +911,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -932,6 +932,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1234,8 +1238,8 @@
   <dimension ref="A1:I48"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:B1"/>
+      <pane ySplit="3" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1251,47 +1255,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="48"/>
-      <c r="B1" s="48"/>
-      <c r="C1" s="66" t="s">
+      <c r="A1" s="78"/>
+      <c r="B1" s="78"/>
+      <c r="C1" s="76" t="s">
+        <v>107</v>
+      </c>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+    </row>
+    <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A2" s="77" t="s">
         <v>108</v>
-      </c>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
-    </row>
-    <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="47" t="s">
-        <v>109</v>
       </c>
       <c r="B2" s="33"/>
       <c r="C2" s="31" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D2" s="31" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E2" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="F2" s="31" t="s">
         <v>98</v>
       </c>
-      <c r="F2" s="31" t="s">
+      <c r="G2" s="31" t="s">
+        <v>101</v>
+      </c>
+      <c r="H2" s="31" t="s">
         <v>99</v>
       </c>
-      <c r="G2" s="31" t="s">
-        <v>102</v>
-      </c>
-      <c r="H2" s="31" t="s">
+      <c r="I2" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="I2" s="31" t="s">
-        <v>101</v>
-      </c>
     </row>
     <row r="3" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="47"/>
+      <c r="A3" s="77"/>
       <c r="B3" s="34"/>
       <c r="C3" s="32" t="s">
         <v>5</v>
@@ -1316,8 +1320,8 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A4" s="47"/>
-      <c r="B4" s="50">
+      <c r="A4" s="77"/>
+      <c r="B4" s="64">
         <v>1</v>
       </c>
       <c r="C4" s="23" t="s">
@@ -1326,48 +1330,48 @@
       <c r="D4" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="49"/>
-      <c r="F4" s="49"/>
-      <c r="G4" s="70" t="s">
+      <c r="E4" s="57"/>
+      <c r="F4" s="57"/>
+      <c r="G4" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="49"/>
+      <c r="H4" s="57"/>
       <c r="I4" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A5" s="47"/>
+      <c r="A5" s="77"/>
       <c r="B5" s="65"/>
       <c r="C5" s="10" t="s">
         <v>22</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="83"/>
-      <c r="H5" s="45"/>
+        <v>111</v>
+      </c>
+      <c r="E5" s="60"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="68"/>
+      <c r="H5" s="60"/>
       <c r="I5" s="21" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="47"/>
-      <c r="B6" s="51"/>
+      <c r="A6" s="77"/>
+      <c r="B6" s="66"/>
       <c r="C6" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="3"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="71"/>
-      <c r="H6" s="46"/>
+      <c r="E6" s="58"/>
+      <c r="F6" s="58"/>
+      <c r="G6" s="69"/>
+      <c r="H6" s="58"/>
       <c r="I6" s="3"/>
     </row>
     <row r="7" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="47"/>
+      <c r="A7" s="77"/>
       <c r="B7" s="35">
         <v>2</v>
       </c>
@@ -1379,12 +1383,12 @@
         <v>12</v>
       </c>
       <c r="H7" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I7" s="4"/>
     </row>
     <row r="8" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="47"/>
+      <c r="A8" s="77"/>
       <c r="B8" s="35">
         <v>3</v>
       </c>
@@ -1401,36 +1405,36 @@
       <c r="I8" s="4"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="47"/>
-      <c r="B9" s="50">
+      <c r="A9" s="77"/>
+      <c r="B9" s="64">
         <v>4</v>
       </c>
-      <c r="C9" s="70" t="s">
+      <c r="C9" s="67" t="s">
         <v>16</v>
       </c>
       <c r="D9" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="49"/>
-      <c r="F9" s="49"/>
-      <c r="G9" s="67"/>
-      <c r="H9" s="72"/>
-      <c r="I9" s="87"/>
+      <c r="E9" s="57"/>
+      <c r="F9" s="57"/>
+      <c r="G9" s="71"/>
+      <c r="H9" s="55"/>
+      <c r="I9" s="47"/>
     </row>
     <row r="10" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="47"/>
-      <c r="B10" s="51"/>
-      <c r="C10" s="71"/>
+      <c r="A10" s="77"/>
+      <c r="B10" s="66"/>
+      <c r="C10" s="69"/>
       <c r="D10" s="12"/>
-      <c r="E10" s="46"/>
-      <c r="F10" s="46"/>
-      <c r="G10" s="69"/>
-      <c r="H10" s="73"/>
-      <c r="I10" s="88"/>
+      <c r="E10" s="58"/>
+      <c r="F10" s="58"/>
+      <c r="G10" s="72"/>
+      <c r="H10" s="56"/>
+      <c r="I10" s="48"/>
     </row>
     <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="47"/>
-      <c r="B11" s="50">
+      <c r="A11" s="77"/>
+      <c r="B11" s="64">
         <v>5</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -1439,37 +1443,37 @@
       <c r="D11" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="49"/>
-      <c r="F11" s="49"/>
-      <c r="G11" s="67" t="s">
+      <c r="E11" s="57"/>
+      <c r="F11" s="57"/>
+      <c r="G11" s="71" t="s">
         <v>18</v>
       </c>
       <c r="H11" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="I11" s="72" t="s">
+      <c r="I11" s="55" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="47"/>
+      <c r="A12" s="77"/>
       <c r="B12" s="65"/>
       <c r="C12" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="45"/>
-      <c r="F12" s="45"/>
-      <c r="G12" s="68"/>
+      <c r="E12" s="60"/>
+      <c r="F12" s="60"/>
+      <c r="G12" s="75"/>
       <c r="H12" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="I12" s="77"/>
+      <c r="I12" s="59"/>
     </row>
     <row r="13" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="47"/>
+      <c r="A13" s="77"/>
       <c r="B13" s="65"/>
       <c r="C13" s="7" t="s">
         <v>26</v>
@@ -1477,14 +1481,14 @@
       <c r="D13" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E13" s="45"/>
-      <c r="F13" s="45"/>
-      <c r="G13" s="68"/>
+      <c r="E13" s="60"/>
+      <c r="F13" s="60"/>
+      <c r="G13" s="75"/>
       <c r="H13" s="39"/>
-      <c r="I13" s="77"/>
+      <c r="I13" s="59"/>
     </row>
     <row r="14" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="47"/>
+      <c r="A14" s="77"/>
       <c r="B14" s="35">
         <v>6</v>
       </c>
@@ -1499,8 +1503,8 @@
       <c r="I14" s="4"/>
     </row>
     <row r="15" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A15" s="47"/>
-      <c r="B15" s="50">
+      <c r="A15" s="77"/>
+      <c r="B15" s="64">
         <v>7</v>
       </c>
       <c r="C15" s="9" t="s">
@@ -1509,16 +1513,16 @@
       <c r="D15" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="49"/>
-      <c r="F15" s="49"/>
-      <c r="G15" s="49"/>
-      <c r="H15" s="72" t="s">
+      <c r="E15" s="57"/>
+      <c r="F15" s="57"/>
+      <c r="G15" s="57"/>
+      <c r="H15" s="55" t="s">
         <v>34</v>
       </c>
-      <c r="I15" s="49"/>
+      <c r="I15" s="57"/>
     </row>
     <row r="16" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A16" s="47"/>
+      <c r="A16" s="77"/>
       <c r="B16" s="65"/>
       <c r="C16" s="19" t="s">
         <v>31</v>
@@ -1526,157 +1530,157 @@
       <c r="D16" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E16" s="45"/>
-      <c r="F16" s="45"/>
-      <c r="G16" s="45"/>
-      <c r="H16" s="77"/>
-      <c r="I16" s="45"/>
+      <c r="E16" s="60"/>
+      <c r="F16" s="60"/>
+      <c r="G16" s="60"/>
+      <c r="H16" s="59"/>
+      <c r="I16" s="60"/>
     </row>
     <row r="17" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="47"/>
-      <c r="B17" s="51"/>
+      <c r="A17" s="77"/>
+      <c r="B17" s="66"/>
       <c r="C17" s="12" t="s">
         <v>33</v>
       </c>
       <c r="D17" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="E17" s="46"/>
-      <c r="F17" s="46"/>
-      <c r="G17" s="46"/>
-      <c r="H17" s="73"/>
-      <c r="I17" s="46"/>
+      <c r="E17" s="58"/>
+      <c r="F17" s="58"/>
+      <c r="G17" s="58"/>
+      <c r="H17" s="56"/>
+      <c r="I17" s="58"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="47"/>
-      <c r="B18" s="50">
+      <c r="A18" s="77"/>
+      <c r="B18" s="64">
         <v>8</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D18" s="67" t="s">
+      <c r="D18" s="71" t="s">
         <v>40</v>
       </c>
-      <c r="E18" s="49"/>
-      <c r="F18" s="49"/>
-      <c r="G18" s="49"/>
-      <c r="H18" s="49"/>
+      <c r="E18" s="57"/>
+      <c r="F18" s="57"/>
+      <c r="G18" s="57"/>
+      <c r="H18" s="57"/>
       <c r="I18" s="6" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A19" s="47"/>
+      <c r="A19" s="77"/>
       <c r="B19" s="65"/>
       <c r="C19" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="D19" s="68"/>
-      <c r="E19" s="45"/>
-      <c r="F19" s="45"/>
-      <c r="G19" s="45"/>
-      <c r="H19" s="45"/>
+      <c r="D19" s="75"/>
+      <c r="E19" s="60"/>
+      <c r="F19" s="60"/>
+      <c r="G19" s="60"/>
+      <c r="H19" s="60"/>
       <c r="I19" s="21" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="47"/>
-      <c r="B20" s="51"/>
+      <c r="A20" s="77"/>
+      <c r="B20" s="66"/>
       <c r="C20" s="3"/>
-      <c r="D20" s="69"/>
-      <c r="E20" s="46"/>
-      <c r="F20" s="46"/>
-      <c r="G20" s="46"/>
-      <c r="H20" s="46"/>
+      <c r="D20" s="72"/>
+      <c r="E20" s="58"/>
+      <c r="F20" s="58"/>
+      <c r="G20" s="58"/>
+      <c r="H20" s="58"/>
       <c r="I20" s="22" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A21" s="47"/>
-      <c r="B21" s="50">
+      <c r="A21" s="77"/>
+      <c r="B21" s="64">
         <v>9</v>
       </c>
       <c r="C21" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="D21" s="70" t="s">
+      <c r="D21" s="67" t="s">
         <v>43</v>
       </c>
-      <c r="E21" s="49"/>
-      <c r="F21" s="67" t="s">
+      <c r="E21" s="57"/>
+      <c r="F21" s="71" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="49"/>
-      <c r="H21" s="74" t="s">
+      <c r="G21" s="57"/>
+      <c r="H21" s="49" t="s">
         <v>41</v>
       </c>
-      <c r="I21" s="49"/>
+      <c r="I21" s="57"/>
     </row>
     <row r="22" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="47"/>
+      <c r="A22" s="77"/>
       <c r="B22" s="65"/>
       <c r="C22" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D22" s="83"/>
-      <c r="E22" s="45"/>
-      <c r="F22" s="68"/>
-      <c r="G22" s="45"/>
-      <c r="H22" s="75"/>
-      <c r="I22" s="45"/>
+      <c r="D22" s="68"/>
+      <c r="E22" s="60"/>
+      <c r="F22" s="75"/>
+      <c r="G22" s="60"/>
+      <c r="H22" s="50"/>
+      <c r="I22" s="60"/>
     </row>
     <row r="23" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="47"/>
-      <c r="B23" s="51"/>
+      <c r="A23" s="77"/>
+      <c r="B23" s="66"/>
       <c r="C23" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="D23" s="71"/>
-      <c r="E23" s="46"/>
-      <c r="F23" s="69"/>
-      <c r="G23" s="46"/>
-      <c r="H23" s="76"/>
-      <c r="I23" s="46"/>
+      <c r="D23" s="69"/>
+      <c r="E23" s="58"/>
+      <c r="F23" s="72"/>
+      <c r="G23" s="58"/>
+      <c r="H23" s="51"/>
+      <c r="I23" s="58"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="47"/>
-      <c r="B24" s="50">
+      <c r="A24" s="77"/>
+      <c r="B24" s="64">
         <v>10</v>
       </c>
-      <c r="C24" s="49"/>
-      <c r="D24" s="49"/>
+      <c r="C24" s="57"/>
+      <c r="D24" s="57"/>
       <c r="E24" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F24" s="67" t="s">
+      <c r="F24" s="71" t="s">
         <v>48</v>
       </c>
-      <c r="G24" s="49"/>
-      <c r="H24" s="49"/>
-      <c r="I24" s="49"/>
+      <c r="G24" s="57"/>
+      <c r="H24" s="57"/>
+      <c r="I24" s="57"/>
     </row>
     <row r="25" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="47"/>
-      <c r="B25" s="51"/>
-      <c r="C25" s="46"/>
-      <c r="D25" s="46"/>
+      <c r="A25" s="77"/>
+      <c r="B25" s="66"/>
+      <c r="C25" s="58"/>
+      <c r="D25" s="58"/>
       <c r="E25" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="F25" s="69"/>
-      <c r="G25" s="46"/>
-      <c r="H25" s="46"/>
-      <c r="I25" s="46"/>
+      <c r="F25" s="72"/>
+      <c r="G25" s="58"/>
+      <c r="H25" s="58"/>
+      <c r="I25" s="58"/>
     </row>
     <row r="26" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="47"/>
+      <c r="A26" s="77"/>
       <c r="B26" s="41">
         <v>11</v>
       </c>
-      <c r="C26" s="89" t="s">
+      <c r="C26" s="45" t="s">
         <v>51</v>
       </c>
       <c r="D26" s="37" t="s">
@@ -1689,96 +1693,96 @@
       <c r="I26" s="2"/>
     </row>
     <row r="27" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A27" s="47"/>
-      <c r="B27" s="50">
+      <c r="A27" s="77"/>
+      <c r="B27" s="64">
         <v>12</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D27" s="74" t="s">
+      <c r="D27" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="E27" s="49"/>
-      <c r="F27" s="84"/>
+      <c r="E27" s="57"/>
+      <c r="F27" s="61"/>
       <c r="G27" s="23" t="s">
         <v>55</v>
       </c>
       <c r="H27" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="I27" s="49"/>
+      <c r="I27" s="57"/>
     </row>
     <row r="28" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A28" s="47"/>
+      <c r="A28" s="77"/>
       <c r="B28" s="65"/>
       <c r="C28" s="21" t="s">
-        <v>114</v>
-      </c>
-      <c r="D28" s="75"/>
-      <c r="E28" s="45"/>
-      <c r="F28" s="85"/>
+        <v>113</v>
+      </c>
+      <c r="D28" s="50"/>
+      <c r="E28" s="60"/>
+      <c r="F28" s="62"/>
       <c r="G28" s="21" t="s">
         <v>56</v>
       </c>
       <c r="H28" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="I28" s="45"/>
+      <c r="I28" s="60"/>
     </row>
     <row r="29" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="47"/>
-      <c r="B29" s="51"/>
+      <c r="A29" s="77"/>
+      <c r="B29" s="66"/>
       <c r="C29" s="3"/>
-      <c r="D29" s="76"/>
-      <c r="E29" s="46"/>
-      <c r="F29" s="86"/>
+      <c r="D29" s="51"/>
+      <c r="E29" s="58"/>
+      <c r="F29" s="63"/>
       <c r="G29" s="14" t="s">
         <v>59</v>
       </c>
       <c r="H29" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="I29" s="46"/>
+      <c r="I29" s="58"/>
     </row>
     <row r="30" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A30" s="47"/>
-      <c r="B30" s="50">
+      <c r="A30" s="77"/>
+      <c r="B30" s="64">
         <v>13</v>
       </c>
       <c r="C30" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="D30" s="67" t="s">
+      <c r="D30" s="71" t="s">
         <v>63</v>
       </c>
-      <c r="E30" s="74" t="s">
+      <c r="E30" s="49" t="s">
         <v>65</v>
       </c>
-      <c r="F30" s="81" t="s">
+      <c r="F30" s="73" t="s">
         <v>64</v>
       </c>
-      <c r="G30" s="49"/>
-      <c r="H30" s="72" t="s">
+      <c r="G30" s="57"/>
+      <c r="H30" s="55" t="s">
         <v>60</v>
       </c>
-      <c r="I30" s="49"/>
+      <c r="I30" s="57"/>
     </row>
     <row r="31" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="47"/>
-      <c r="B31" s="51"/>
+      <c r="A31" s="77"/>
+      <c r="B31" s="66"/>
       <c r="C31" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="D31" s="69"/>
-      <c r="E31" s="76"/>
-      <c r="F31" s="82"/>
-      <c r="G31" s="46"/>
-      <c r="H31" s="73"/>
-      <c r="I31" s="46"/>
+      <c r="D31" s="72"/>
+      <c r="E31" s="51"/>
+      <c r="F31" s="74"/>
+      <c r="G31" s="58"/>
+      <c r="H31" s="56"/>
+      <c r="I31" s="58"/>
     </row>
     <row r="32" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="47"/>
+      <c r="A32" s="77"/>
       <c r="B32" s="35">
         <v>14</v>
       </c>
@@ -1795,7 +1799,7 @@
       <c r="I32" s="5"/>
     </row>
     <row r="33" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="47"/>
+      <c r="A33" s="77"/>
       <c r="B33" s="35">
         <v>15</v>
       </c>
@@ -1814,68 +1818,68 @@
       <c r="I33" s="5"/>
     </row>
     <row r="34" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A34" s="47"/>
-      <c r="B34" s="50">
+      <c r="A34" s="77"/>
+      <c r="B34" s="64">
         <v>16</v>
       </c>
       <c r="C34" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="D34" s="74" t="s">
+      <c r="D34" s="49" t="s">
         <v>71</v>
       </c>
-      <c r="E34" s="84"/>
-      <c r="F34" s="49"/>
-      <c r="G34" s="49"/>
+      <c r="E34" s="61"/>
+      <c r="F34" s="57"/>
+      <c r="G34" s="57"/>
       <c r="H34" s="38" t="s">
         <v>74</v>
       </c>
-      <c r="I34" s="72" t="s">
+      <c r="I34" s="55" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="47"/>
+      <c r="A35" s="77"/>
       <c r="B35" s="65"/>
       <c r="C35" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="D35" s="75"/>
-      <c r="E35" s="85"/>
-      <c r="F35" s="45"/>
-      <c r="G35" s="45"/>
+      <c r="D35" s="50"/>
+      <c r="E35" s="62"/>
+      <c r="F35" s="60"/>
+      <c r="G35" s="60"/>
       <c r="H35" s="44" t="s">
-        <v>111</v>
-      </c>
-      <c r="I35" s="77"/>
+        <v>110</v>
+      </c>
+      <c r="I35" s="59"/>
     </row>
     <row r="36" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="47"/>
-      <c r="B36" s="51"/>
+      <c r="A36" s="77"/>
+      <c r="B36" s="66"/>
       <c r="C36" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="D36" s="76"/>
-      <c r="E36" s="86"/>
-      <c r="F36" s="46"/>
-      <c r="G36" s="46"/>
-      <c r="H36" s="90"/>
-      <c r="I36" s="73"/>
+      <c r="D36" s="51"/>
+      <c r="E36" s="63"/>
+      <c r="F36" s="58"/>
+      <c r="G36" s="58"/>
+      <c r="H36" s="46"/>
+      <c r="I36" s="56"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37" s="47"/>
-      <c r="B37" s="50">
+      <c r="A37" s="77"/>
+      <c r="B37" s="64">
         <v>17</v>
       </c>
       <c r="C37" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="D37" s="59" t="s">
+      <c r="D37" s="85" t="s">
         <v>84</v>
       </c>
-      <c r="E37" s="49"/>
-      <c r="F37" s="49"/>
-      <c r="G37" s="62" t="s">
+      <c r="E37" s="57"/>
+      <c r="F37" s="57"/>
+      <c r="G37" s="88" t="s">
         <v>83</v>
       </c>
       <c r="H37" s="42" t="s">
@@ -1886,15 +1890,15 @@
       </c>
     </row>
     <row r="38" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A38" s="47"/>
+      <c r="A38" s="77"/>
       <c r="B38" s="65"/>
       <c r="C38" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="D38" s="60"/>
-      <c r="E38" s="45"/>
-      <c r="F38" s="45"/>
-      <c r="G38" s="63"/>
+        <v>115</v>
+      </c>
+      <c r="D38" s="86"/>
+      <c r="E38" s="60"/>
+      <c r="F38" s="60"/>
+      <c r="G38" s="89"/>
       <c r="H38" s="43" t="s">
         <v>79</v>
       </c>
@@ -1903,88 +1907,88 @@
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A39" s="47"/>
+      <c r="A39" s="77"/>
       <c r="B39" s="65"/>
       <c r="C39" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="D39" s="60"/>
-      <c r="E39" s="45"/>
-      <c r="F39" s="45"/>
-      <c r="G39" s="63"/>
-      <c r="H39" s="45"/>
-      <c r="I39" s="45"/>
+      <c r="D39" s="86"/>
+      <c r="E39" s="60"/>
+      <c r="F39" s="60"/>
+      <c r="G39" s="89"/>
+      <c r="H39" s="60"/>
+      <c r="I39" s="60"/>
     </row>
     <row r="40" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="47"/>
-      <c r="B40" s="51"/>
+      <c r="A40" s="77"/>
+      <c r="B40" s="66"/>
       <c r="C40" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="D40" s="61"/>
-      <c r="E40" s="46"/>
-      <c r="F40" s="46"/>
-      <c r="G40" s="64"/>
-      <c r="H40" s="46"/>
-      <c r="I40" s="46"/>
+      <c r="D40" s="87"/>
+      <c r="E40" s="58"/>
+      <c r="F40" s="58"/>
+      <c r="G40" s="90"/>
+      <c r="H40" s="58"/>
+      <c r="I40" s="58"/>
     </row>
     <row r="41" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A41" s="47"/>
-      <c r="B41" s="50">
+      <c r="A41" s="77"/>
+      <c r="B41" s="64">
         <v>18</v>
       </c>
-      <c r="C41" s="49"/>
+      <c r="C41" s="57"/>
       <c r="D41" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="E41" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="F41" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="G41" s="57"/>
+      <c r="H41" s="52" t="s">
+        <v>95</v>
+      </c>
+      <c r="I41" s="52" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A42" s="77"/>
+      <c r="B42" s="65"/>
+      <c r="C42" s="60"/>
+      <c r="D42" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="E41" s="20" t="s">
+      <c r="E42" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="F42" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="F41" s="20" t="s">
-        <v>87</v>
-      </c>
-      <c r="G41" s="49"/>
-      <c r="H41" s="78" t="s">
-        <v>96</v>
-      </c>
-      <c r="I41" s="78" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A42" s="47"/>
-      <c r="B42" s="65"/>
-      <c r="C42" s="45"/>
-      <c r="D42" s="19" t="s">
-        <v>95</v>
-      </c>
-      <c r="E42" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="F42" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="G42" s="45"/>
-      <c r="H42" s="79"/>
-      <c r="I42" s="79"/>
+      <c r="G42" s="60"/>
+      <c r="H42" s="53"/>
+      <c r="I42" s="53"/>
     </row>
     <row r="43" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="47"/>
-      <c r="B43" s="51"/>
-      <c r="C43" s="46"/>
+      <c r="A43" s="77"/>
+      <c r="B43" s="66"/>
+      <c r="C43" s="58"/>
       <c r="D43" s="3"/>
       <c r="E43" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F43" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="G43" s="46"/>
-      <c r="H43" s="80"/>
-      <c r="I43" s="80"/>
+        <v>91</v>
+      </c>
+      <c r="G43" s="58"/>
+      <c r="H43" s="54"/>
+      <c r="I43" s="54"/>
     </row>
     <row r="44" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="47"/>
+      <c r="A44" s="77"/>
       <c r="B44" s="35">
         <v>20</v>
       </c>
@@ -1994,27 +1998,27 @@
       <c r="F44" s="5"/>
       <c r="G44" s="5"/>
       <c r="H44" s="15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I44" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="48"/>
-      <c r="B45" s="57" t="s">
-        <v>107</v>
-      </c>
-      <c r="C45" s="57"/>
-      <c r="D45" s="57"/>
-      <c r="E45" s="57"/>
-      <c r="F45" s="57"/>
-      <c r="G45" s="57"/>
-      <c r="H45" s="57"/>
-      <c r="I45" s="58"/>
+      <c r="A45" s="78"/>
+      <c r="B45" s="70" t="s">
+        <v>106</v>
+      </c>
+      <c r="C45" s="70"/>
+      <c r="D45" s="70"/>
+      <c r="E45" s="70"/>
+      <c r="F45" s="70"/>
+      <c r="G45" s="70"/>
+      <c r="H45" s="70"/>
+      <c r="I45" s="84"/>
     </row>
     <row r="46" spans="1:9" s="16" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="48"/>
+      <c r="A46" s="78"/>
       <c r="B46" s="18"/>
       <c r="C46" s="17">
         <f t="shared" ref="C46:I46" si="0">COUNTIF(C4:C44, "&lt;&gt;")</f>
@@ -2046,55 +2050,69 @@
       </c>
     </row>
     <row r="47" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="48"/>
-      <c r="B47" s="57" t="str">
+      <c r="A47" s="78"/>
+      <c r="B47" s="70" t="str">
         <f>SUM(C46:I46) &amp; " Total Races (Prior to Breeders' Cup Weekend)"</f>
         <v>98 Total Races (Prior to Breeders' Cup Weekend)</v>
       </c>
-      <c r="C47" s="57"/>
-      <c r="D47" s="57"/>
-      <c r="E47" s="57"/>
-      <c r="F47" s="57"/>
-      <c r="G47" s="57"/>
-      <c r="H47" s="57"/>
-      <c r="I47" s="57"/>
+      <c r="C47" s="70"/>
+      <c r="D47" s="70"/>
+      <c r="E47" s="70"/>
+      <c r="F47" s="70"/>
+      <c r="G47" s="70"/>
+      <c r="H47" s="70"/>
+      <c r="I47" s="70"/>
     </row>
     <row r="48" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="48"/>
-      <c r="B48" s="52" t="s">
+      <c r="A48" s="78"/>
+      <c r="B48" s="79" t="s">
+        <v>104</v>
+      </c>
+      <c r="C48" s="79"/>
+      <c r="D48" s="79"/>
+      <c r="E48" s="80"/>
+      <c r="F48" s="81" t="s">
         <v>105</v>
       </c>
-      <c r="C48" s="52"/>
-      <c r="D48" s="52"/>
-      <c r="E48" s="53"/>
-      <c r="F48" s="54" t="s">
-        <v>106</v>
-      </c>
-      <c r="G48" s="55"/>
-      <c r="H48" s="55"/>
-      <c r="I48" s="56"/>
+      <c r="G48" s="82"/>
+      <c r="H48" s="82"/>
+      <c r="I48" s="83"/>
     </row>
   </sheetData>
   <mergeCells count="81">
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="D34:D36"/>
-    <mergeCell ref="H41:H43"/>
-    <mergeCell ref="H30:H31"/>
-    <mergeCell ref="I30:I31"/>
-    <mergeCell ref="D27:D29"/>
-    <mergeCell ref="I34:I36"/>
-    <mergeCell ref="G34:G36"/>
-    <mergeCell ref="F34:F36"/>
-    <mergeCell ref="E34:E36"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="G4:G6"/>
-    <mergeCell ref="I27:I29"/>
-    <mergeCell ref="F27:F29"/>
-    <mergeCell ref="E27:E29"/>
-    <mergeCell ref="I24:I25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="I41:I43"/>
+    <mergeCell ref="I39:I40"/>
+    <mergeCell ref="A2:A44"/>
+    <mergeCell ref="A45:A48"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="E4:E6"/>
+    <mergeCell ref="F4:F6"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B48:E48"/>
+    <mergeCell ref="F48:I48"/>
+    <mergeCell ref="B45:I45"/>
+    <mergeCell ref="D37:D40"/>
+    <mergeCell ref="E37:E40"/>
+    <mergeCell ref="F37:F40"/>
+    <mergeCell ref="G37:G40"/>
+    <mergeCell ref="B37:B40"/>
+    <mergeCell ref="C1:I1"/>
+    <mergeCell ref="E15:E17"/>
+    <mergeCell ref="I11:I13"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="E11:E13"/>
+    <mergeCell ref="F11:F13"/>
+    <mergeCell ref="G11:G13"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="G15:G17"/>
+    <mergeCell ref="F15:F17"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="C41:C43"/>
+    <mergeCell ref="H4:H6"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="H21:H23"/>
+    <mergeCell ref="H39:H40"/>
     <mergeCell ref="B47:I47"/>
     <mergeCell ref="G41:G43"/>
     <mergeCell ref="B4:B6"/>
@@ -2111,6 +2129,14 @@
     <mergeCell ref="B18:B20"/>
     <mergeCell ref="D18:D20"/>
     <mergeCell ref="C24:C25"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="G4:G6"/>
+    <mergeCell ref="I27:I29"/>
+    <mergeCell ref="F27:F29"/>
+    <mergeCell ref="E27:E29"/>
+    <mergeCell ref="I24:I25"/>
+    <mergeCell ref="B24:B25"/>
     <mergeCell ref="D24:D25"/>
     <mergeCell ref="F24:F25"/>
     <mergeCell ref="G24:G25"/>
@@ -2119,44 +2145,22 @@
     <mergeCell ref="G21:G23"/>
     <mergeCell ref="E21:E23"/>
     <mergeCell ref="I15:I17"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="D34:D36"/>
+    <mergeCell ref="H41:H43"/>
+    <mergeCell ref="H30:H31"/>
+    <mergeCell ref="I30:I31"/>
+    <mergeCell ref="D27:D29"/>
+    <mergeCell ref="I34:I36"/>
+    <mergeCell ref="G34:G36"/>
+    <mergeCell ref="F34:F36"/>
+    <mergeCell ref="E34:E36"/>
+    <mergeCell ref="I41:I43"/>
     <mergeCell ref="H18:H20"/>
     <mergeCell ref="G18:G20"/>
     <mergeCell ref="F18:F20"/>
     <mergeCell ref="E18:E20"/>
     <mergeCell ref="H15:H17"/>
-    <mergeCell ref="G15:G17"/>
-    <mergeCell ref="F15:F17"/>
-    <mergeCell ref="B41:B43"/>
-    <mergeCell ref="C41:C43"/>
-    <mergeCell ref="H4:H6"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="C1:I1"/>
-    <mergeCell ref="E15:E17"/>
-    <mergeCell ref="I11:I13"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="E11:E13"/>
-    <mergeCell ref="F11:F13"/>
-    <mergeCell ref="G11:G13"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="H21:H23"/>
-    <mergeCell ref="H39:H40"/>
-    <mergeCell ref="I39:I40"/>
-    <mergeCell ref="A2:A44"/>
-    <mergeCell ref="A45:A48"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="E4:E6"/>
-    <mergeCell ref="F4:F6"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B48:E48"/>
-    <mergeCell ref="F48:I48"/>
-    <mergeCell ref="B45:I45"/>
-    <mergeCell ref="D37:D40"/>
-    <mergeCell ref="E37:E40"/>
-    <mergeCell ref="F37:F40"/>
-    <mergeCell ref="G37:G40"/>
-    <mergeCell ref="B37:B40"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
RTTBC24 Week 9 Noms (DMR, MNR), Week 10 (SAR);  Week 9 Entries SAR
</commit_message>
<xml_diff>
--- a/pdf/RTTBC24-Schedule-by-Division.xlsx
+++ b/pdf/RTTBC24-Schedule-by-Division.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/299f8723705ec823/Webmaster/gallop-racing.com/pdf/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1123" documentId="8_{DAECCBE5-FF72-4188-B2F1-1541968A3FDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4D62769E-C4E0-45ED-BEF2-6D1B832643D9}"/>
+  <xr:revisionPtr revIDLastSave="1124" documentId="8_{DAECCBE5-FF72-4188-B2F1-1541968A3FDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1553D2E4-EEE3-4355-A495-CD3DDB4F8175}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{EAD27B02-19FE-4D48-9014-ED6E24DB84F0}"/>
   </bookViews>
@@ -161,9 +161,6 @@
     <t>Monmouth Oaks-G3</t>
   </si>
   <si>
-    <t>Longines Test S.-G1</t>
-  </si>
-  <si>
     <t>Whitney H.-G1</t>
   </si>
   <si>
@@ -384,6 +381,9 @@
   </si>
   <si>
     <t>California Crown S.-G1</t>
+  </si>
+  <si>
+    <t>Test S.-G1</t>
   </si>
 </sst>
 </file>
@@ -786,11 +786,98 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
@@ -798,15 +885,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -822,9 +900,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -840,83 +915,8 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1244,8 +1244,8 @@
   <dimension ref="A1:I47"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E42" sqref="E42"/>
+      <pane ySplit="3" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H21" sqref="H21:H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1261,47 +1261,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="50"/>
-      <c r="B1" s="50"/>
-      <c r="C1" s="66" t="s">
+      <c r="A1" s="79"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="90" t="s">
+        <v>106</v>
+      </c>
+      <c r="D1" s="90"/>
+      <c r="E1" s="90"/>
+      <c r="F1" s="90"/>
+      <c r="G1" s="90"/>
+      <c r="H1" s="90"/>
+      <c r="I1" s="90"/>
+    </row>
+    <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A2" s="78" t="s">
         <v>107</v>
-      </c>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
-    </row>
-    <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="49" t="s">
-        <v>108</v>
       </c>
       <c r="B2" s="33"/>
       <c r="C2" s="31" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D2" s="31" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E2" s="31" t="s">
+        <v>96</v>
+      </c>
+      <c r="F2" s="31" t="s">
         <v>97</v>
       </c>
-      <c r="F2" s="31" t="s">
+      <c r="G2" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="H2" s="31" t="s">
         <v>98</v>
       </c>
-      <c r="G2" s="31" t="s">
-        <v>101</v>
-      </c>
-      <c r="H2" s="31" t="s">
+      <c r="I2" s="31" t="s">
         <v>99</v>
       </c>
-      <c r="I2" s="31" t="s">
-        <v>100</v>
-      </c>
     </row>
     <row r="3" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="49"/>
+      <c r="A3" s="78"/>
       <c r="B3" s="34"/>
       <c r="C3" s="32" t="s">
         <v>5</v>
@@ -1326,8 +1326,8 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A4" s="49"/>
-      <c r="B4" s="52">
+      <c r="A4" s="78"/>
+      <c r="B4" s="66">
         <v>1</v>
       </c>
       <c r="C4" s="23" t="s">
@@ -1336,48 +1336,48 @@
       <c r="D4" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="51"/>
-      <c r="F4" s="51"/>
-      <c r="G4" s="69" t="s">
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="74" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="51"/>
+      <c r="H4" s="52"/>
       <c r="I4" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A5" s="49"/>
-      <c r="B5" s="65"/>
+      <c r="A5" s="78"/>
+      <c r="B5" s="71"/>
       <c r="C5" s="10" t="s">
         <v>22</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="E5" s="47"/>
-      <c r="F5" s="47"/>
-      <c r="G5" s="80"/>
-      <c r="H5" s="47"/>
+        <v>110</v>
+      </c>
+      <c r="E5" s="53"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="75"/>
+      <c r="H5" s="53"/>
       <c r="I5" s="21" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="49"/>
-      <c r="B6" s="53"/>
+      <c r="A6" s="78"/>
+      <c r="B6" s="67"/>
       <c r="C6" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="3"/>
-      <c r="E6" s="48"/>
-      <c r="F6" s="48"/>
-      <c r="G6" s="70"/>
-      <c r="H6" s="48"/>
+      <c r="E6" s="54"/>
+      <c r="F6" s="54"/>
+      <c r="G6" s="76"/>
+      <c r="H6" s="54"/>
       <c r="I6" s="3"/>
     </row>
     <row r="7" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="49"/>
+      <c r="A7" s="78"/>
       <c r="B7" s="35">
         <v>2</v>
       </c>
@@ -1389,12 +1389,12 @@
         <v>12</v>
       </c>
       <c r="H7" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I7" s="4"/>
     </row>
     <row r="8" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="49"/>
+      <c r="A8" s="78"/>
       <c r="B8" s="35">
         <v>3</v>
       </c>
@@ -1411,36 +1411,36 @@
       <c r="I8" s="4"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="49"/>
-      <c r="B9" s="52">
+      <c r="A9" s="78"/>
+      <c r="B9" s="66">
         <v>4</v>
       </c>
-      <c r="C9" s="69" t="s">
+      <c r="C9" s="74" t="s">
         <v>16</v>
       </c>
       <c r="D9" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="51"/>
-      <c r="F9" s="51"/>
-      <c r="G9" s="71"/>
-      <c r="H9" s="67"/>
-      <c r="I9" s="84"/>
+      <c r="E9" s="52"/>
+      <c r="F9" s="52"/>
+      <c r="G9" s="68"/>
+      <c r="H9" s="55"/>
+      <c r="I9" s="64"/>
     </row>
     <row r="10" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="49"/>
-      <c r="B10" s="53"/>
-      <c r="C10" s="70"/>
+      <c r="A10" s="78"/>
+      <c r="B10" s="67"/>
+      <c r="C10" s="76"/>
       <c r="D10" s="12"/>
-      <c r="E10" s="48"/>
-      <c r="F10" s="48"/>
-      <c r="G10" s="72"/>
-      <c r="H10" s="73"/>
-      <c r="I10" s="85"/>
+      <c r="E10" s="54"/>
+      <c r="F10" s="54"/>
+      <c r="G10" s="69"/>
+      <c r="H10" s="60"/>
+      <c r="I10" s="65"/>
     </row>
     <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="49"/>
-      <c r="B11" s="52">
+      <c r="A11" s="78"/>
+      <c r="B11" s="66">
         <v>5</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -1449,52 +1449,52 @@
       <c r="D11" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="51"/>
-      <c r="F11" s="51"/>
-      <c r="G11" s="71" t="s">
+      <c r="E11" s="52"/>
+      <c r="F11" s="52"/>
+      <c r="G11" s="68" t="s">
         <v>18</v>
       </c>
       <c r="H11" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="I11" s="67" t="s">
+      <c r="I11" s="55" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="49"/>
-      <c r="B12" s="65"/>
+      <c r="A12" s="78"/>
+      <c r="B12" s="71"/>
       <c r="C12" s="10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="47"/>
-      <c r="F12" s="47"/>
-      <c r="G12" s="74"/>
+      <c r="E12" s="53"/>
+      <c r="F12" s="53"/>
+      <c r="G12" s="77"/>
       <c r="H12" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="I12" s="68"/>
+      <c r="I12" s="56"/>
     </row>
     <row r="13" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="49"/>
-      <c r="B13" s="65"/>
+      <c r="A13" s="78"/>
+      <c r="B13" s="71"/>
       <c r="C13" s="7" t="s">
         <v>26</v>
       </c>
       <c r="D13" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E13" s="47"/>
-      <c r="F13" s="47"/>
-      <c r="G13" s="74"/>
+      <c r="E13" s="53"/>
+      <c r="F13" s="53"/>
+      <c r="G13" s="77"/>
       <c r="H13" s="39"/>
-      <c r="I13" s="68"/>
+      <c r="I13" s="56"/>
     </row>
     <row r="14" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="49"/>
+      <c r="A14" s="78"/>
       <c r="B14" s="35">
         <v>6</v>
       </c>
@@ -1509,8 +1509,8 @@
       <c r="I14" s="4"/>
     </row>
     <row r="15" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A15" s="49"/>
-      <c r="B15" s="52">
+      <c r="A15" s="78"/>
+      <c r="B15" s="66">
         <v>7</v>
       </c>
       <c r="C15" s="9" t="s">
@@ -1519,178 +1519,178 @@
       <c r="D15" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="51"/>
-      <c r="F15" s="51"/>
-      <c r="G15" s="51"/>
-      <c r="H15" s="67" t="s">
+      <c r="E15" s="52"/>
+      <c r="F15" s="52"/>
+      <c r="G15" s="52"/>
+      <c r="H15" s="55" t="s">
         <v>34</v>
       </c>
-      <c r="I15" s="51"/>
+      <c r="I15" s="52"/>
     </row>
     <row r="16" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A16" s="49"/>
-      <c r="B16" s="65"/>
+      <c r="A16" s="78"/>
+      <c r="B16" s="71"/>
       <c r="C16" s="19" t="s">
         <v>31</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E16" s="47"/>
-      <c r="F16" s="47"/>
-      <c r="G16" s="47"/>
-      <c r="H16" s="68"/>
-      <c r="I16" s="47"/>
+      <c r="E16" s="53"/>
+      <c r="F16" s="53"/>
+      <c r="G16" s="53"/>
+      <c r="H16" s="56"/>
+      <c r="I16" s="53"/>
     </row>
     <row r="17" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="49"/>
-      <c r="B17" s="53"/>
+      <c r="A17" s="78"/>
+      <c r="B17" s="67"/>
       <c r="C17" s="12" t="s">
         <v>33</v>
       </c>
       <c r="D17" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="E17" s="48"/>
-      <c r="F17" s="48"/>
-      <c r="G17" s="48"/>
-      <c r="H17" s="73"/>
-      <c r="I17" s="48"/>
+      <c r="E17" s="54"/>
+      <c r="F17" s="54"/>
+      <c r="G17" s="54"/>
+      <c r="H17" s="60"/>
+      <c r="I17" s="54"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="49"/>
-      <c r="B18" s="52">
+      <c r="A18" s="78"/>
+      <c r="B18" s="66">
         <v>8</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D18" s="71" t="s">
+      <c r="D18" s="68" t="s">
         <v>40</v>
       </c>
-      <c r="E18" s="51"/>
-      <c r="F18" s="51"/>
-      <c r="G18" s="51"/>
-      <c r="H18" s="51"/>
+      <c r="E18" s="52"/>
+      <c r="F18" s="52"/>
+      <c r="G18" s="52"/>
+      <c r="H18" s="52"/>
       <c r="I18" s="6" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A19" s="49"/>
-      <c r="B19" s="65"/>
+      <c r="A19" s="78"/>
+      <c r="B19" s="71"/>
       <c r="C19" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="D19" s="74"/>
-      <c r="E19" s="47"/>
-      <c r="F19" s="47"/>
-      <c r="G19" s="47"/>
-      <c r="H19" s="47"/>
+      <c r="D19" s="77"/>
+      <c r="E19" s="53"/>
+      <c r="F19" s="53"/>
+      <c r="G19" s="53"/>
+      <c r="H19" s="53"/>
       <c r="I19" s="21" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="49"/>
-      <c r="B20" s="53"/>
+      <c r="A20" s="78"/>
+      <c r="B20" s="67"/>
       <c r="C20" s="3"/>
-      <c r="D20" s="72"/>
-      <c r="E20" s="48"/>
-      <c r="F20" s="48"/>
-      <c r="G20" s="48"/>
-      <c r="H20" s="48"/>
+      <c r="D20" s="69"/>
+      <c r="E20" s="54"/>
+      <c r="F20" s="54"/>
+      <c r="G20" s="54"/>
+      <c r="H20" s="54"/>
       <c r="I20" s="22" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A21" s="49"/>
-      <c r="B21" s="52">
+      <c r="A21" s="78"/>
+      <c r="B21" s="66">
         <v>9</v>
       </c>
       <c r="C21" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" s="74" t="s">
         <v>42</v>
       </c>
-      <c r="D21" s="69" t="s">
+      <c r="E21" s="52"/>
+      <c r="F21" s="68" t="s">
+        <v>45</v>
+      </c>
+      <c r="G21" s="52"/>
+      <c r="H21" s="57" t="s">
+        <v>115</v>
+      </c>
+      <c r="I21" s="52"/>
+    </row>
+    <row r="22" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="78"/>
+      <c r="B22" s="71"/>
+      <c r="C22" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E21" s="51"/>
-      <c r="F21" s="71" t="s">
+      <c r="D22" s="75"/>
+      <c r="E22" s="53"/>
+      <c r="F22" s="77"/>
+      <c r="G22" s="53"/>
+      <c r="H22" s="58"/>
+      <c r="I22" s="53"/>
+    </row>
+    <row r="23" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="78"/>
+      <c r="B23" s="67"/>
+      <c r="C23" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" s="76"/>
+      <c r="E23" s="54"/>
+      <c r="F23" s="69"/>
+      <c r="G23" s="54"/>
+      <c r="H23" s="59"/>
+      <c r="I23" s="54"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="78"/>
+      <c r="B24" s="66">
+        <v>10</v>
+      </c>
+      <c r="C24" s="52"/>
+      <c r="D24" s="52"/>
+      <c r="E24" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="51"/>
-      <c r="H21" s="75" t="s">
-        <v>41</v>
-      </c>
-      <c r="I21" s="51"/>
-    </row>
-    <row r="22" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="49"/>
-      <c r="B22" s="65"/>
-      <c r="C22" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D22" s="80"/>
-      <c r="E22" s="47"/>
-      <c r="F22" s="74"/>
-      <c r="G22" s="47"/>
-      <c r="H22" s="76"/>
-      <c r="I22" s="47"/>
-    </row>
-    <row r="23" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="49"/>
-      <c r="B23" s="53"/>
-      <c r="C23" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="D23" s="70"/>
-      <c r="E23" s="48"/>
-      <c r="F23" s="72"/>
-      <c r="G23" s="48"/>
-      <c r="H23" s="77"/>
-      <c r="I23" s="48"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="49"/>
-      <c r="B24" s="52">
-        <v>10</v>
-      </c>
-      <c r="C24" s="51"/>
-      <c r="D24" s="51"/>
-      <c r="E24" s="6" t="s">
+      <c r="F24" s="68" t="s">
         <v>47</v>
       </c>
-      <c r="F24" s="71" t="s">
+      <c r="G24" s="52"/>
+      <c r="H24" s="52"/>
+      <c r="I24" s="52"/>
+    </row>
+    <row r="25" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="78"/>
+      <c r="B25" s="67"/>
+      <c r="C25" s="54"/>
+      <c r="D25" s="54"/>
+      <c r="E25" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="G24" s="51"/>
-      <c r="H24" s="51"/>
-      <c r="I24" s="51"/>
-    </row>
-    <row r="25" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="49"/>
-      <c r="B25" s="53"/>
-      <c r="C25" s="48"/>
-      <c r="D25" s="48"/>
-      <c r="E25" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="F25" s="72"/>
-      <c r="G25" s="48"/>
-      <c r="H25" s="48"/>
-      <c r="I25" s="48"/>
+      <c r="F25" s="69"/>
+      <c r="G25" s="54"/>
+      <c r="H25" s="54"/>
+      <c r="I25" s="54"/>
     </row>
     <row r="26" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="49"/>
+      <c r="A26" s="78"/>
       <c r="B26" s="41">
         <v>11</v>
       </c>
       <c r="C26" s="44" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D26" s="37" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
@@ -1699,291 +1699,291 @@
       <c r="I26" s="2"/>
     </row>
     <row r="27" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A27" s="49"/>
-      <c r="B27" s="52">
+      <c r="A27" s="78"/>
+      <c r="B27" s="66">
         <v>12</v>
       </c>
       <c r="C27" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D27" s="57" t="s">
+        <v>53</v>
+      </c>
+      <c r="E27" s="52"/>
+      <c r="F27" s="61"/>
+      <c r="G27" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="H27" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="I27" s="52"/>
+    </row>
+    <row r="28" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A28" s="78"/>
+      <c r="B28" s="71"/>
+      <c r="C28" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="D28" s="58"/>
+      <c r="E28" s="53"/>
+      <c r="F28" s="62"/>
+      <c r="G28" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="H28" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="I28" s="53"/>
+    </row>
+    <row r="29" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="78"/>
+      <c r="B29" s="67"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="59"/>
+      <c r="E29" s="54"/>
+      <c r="F29" s="63"/>
+      <c r="G29" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="H29" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="D27" s="75" t="s">
-        <v>54</v>
-      </c>
-      <c r="E27" s="51"/>
-      <c r="F27" s="81"/>
-      <c r="G27" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="H27" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="I27" s="51"/>
-    </row>
-    <row r="28" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A28" s="49"/>
-      <c r="B28" s="65"/>
-      <c r="C28" s="21" t="s">
-        <v>113</v>
-      </c>
-      <c r="D28" s="76"/>
-      <c r="E28" s="47"/>
-      <c r="F28" s="82"/>
-      <c r="G28" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="H28" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="I28" s="47"/>
-    </row>
-    <row r="29" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="49"/>
-      <c r="B29" s="53"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="77"/>
-      <c r="E29" s="48"/>
-      <c r="F29" s="83"/>
-      <c r="G29" s="14" t="s">
+      <c r="I29" s="54"/>
+    </row>
+    <row r="30" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A30" s="78"/>
+      <c r="B30" s="66">
+        <v>13</v>
+      </c>
+      <c r="C30" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="D30" s="68" t="s">
+        <v>62</v>
+      </c>
+      <c r="E30" s="57" t="s">
+        <v>64</v>
+      </c>
+      <c r="F30" s="72" t="s">
+        <v>63</v>
+      </c>
+      <c r="G30" s="52"/>
+      <c r="H30" s="55" t="s">
         <v>59</v>
       </c>
-      <c r="H29" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="I29" s="48"/>
-    </row>
-    <row r="30" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A30" s="49"/>
-      <c r="B30" s="52">
-        <v>13</v>
-      </c>
-      <c r="C30" s="20" t="s">
+      <c r="I30" s="52"/>
+    </row>
+    <row r="31" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A31" s="78"/>
+      <c r="B31" s="67"/>
+      <c r="C31" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="D30" s="71" t="s">
-        <v>63</v>
-      </c>
-      <c r="E30" s="75" t="s">
-        <v>65</v>
-      </c>
-      <c r="F30" s="78" t="s">
-        <v>64</v>
-      </c>
-      <c r="G30" s="51"/>
-      <c r="H30" s="67" t="s">
-        <v>60</v>
-      </c>
-      <c r="I30" s="51"/>
-    </row>
-    <row r="31" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="49"/>
-      <c r="B31" s="53"/>
-      <c r="C31" s="22" t="s">
-        <v>62</v>
-      </c>
-      <c r="D31" s="72"/>
-      <c r="E31" s="77"/>
-      <c r="F31" s="79"/>
-      <c r="G31" s="48"/>
-      <c r="H31" s="73"/>
-      <c r="I31" s="48"/>
+      <c r="D31" s="69"/>
+      <c r="E31" s="59"/>
+      <c r="F31" s="73"/>
+      <c r="G31" s="54"/>
+      <c r="H31" s="60"/>
+      <c r="I31" s="54"/>
     </row>
     <row r="32" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="49"/>
+      <c r="A32" s="78"/>
       <c r="B32" s="35">
         <v>14</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
       <c r="E32" s="27" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F32" s="28" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G32" s="5"/>
       <c r="H32" s="5"/>
       <c r="I32" s="5"/>
     </row>
     <row r="33" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="49"/>
+      <c r="A33" s="78"/>
       <c r="B33" s="35">
         <v>15</v>
       </c>
       <c r="C33" s="5"/>
       <c r="D33" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E33" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="F33" s="30" t="s">
         <v>68</v>
-      </c>
-      <c r="F33" s="30" t="s">
-        <v>69</v>
       </c>
       <c r="G33" s="5"/>
       <c r="H33" s="5"/>
       <c r="I33" s="5"/>
     </row>
     <row r="34" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A34" s="49"/>
-      <c r="B34" s="52">
+      <c r="A34" s="78"/>
+      <c r="B34" s="66">
         <v>16</v>
       </c>
       <c r="C34" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="D34" s="57" t="s">
+        <v>70</v>
+      </c>
+      <c r="E34" s="61"/>
+      <c r="F34" s="52"/>
+      <c r="G34" s="52"/>
+      <c r="H34" s="38" t="s">
+        <v>73</v>
+      </c>
+      <c r="I34" s="55" t="s">
         <v>72</v>
       </c>
-      <c r="D34" s="75" t="s">
-        <v>71</v>
-      </c>
-      <c r="E34" s="81"/>
-      <c r="F34" s="51"/>
-      <c r="G34" s="51"/>
-      <c r="H34" s="38" t="s">
+    </row>
+    <row r="35" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="78"/>
+      <c r="B35" s="71"/>
+      <c r="C35" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="I34" s="67" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="49"/>
-      <c r="B35" s="65"/>
-      <c r="C35" s="7" t="s">
+      <c r="D35" s="58"/>
+      <c r="E35" s="62"/>
+      <c r="F35" s="53"/>
+      <c r="G35" s="53"/>
+      <c r="H35" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="I35" s="56"/>
+    </row>
+    <row r="36" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="78"/>
+      <c r="B36" s="67"/>
+      <c r="C36" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="D35" s="76"/>
-      <c r="E35" s="82"/>
-      <c r="F35" s="47"/>
-      <c r="G35" s="47"/>
-      <c r="H35" s="43" t="s">
-        <v>110</v>
-      </c>
-      <c r="I35" s="68"/>
-    </row>
-    <row r="36" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="49"/>
-      <c r="B36" s="53"/>
-      <c r="C36" s="12" t="s">
+      <c r="D36" s="59"/>
+      <c r="E36" s="63"/>
+      <c r="F36" s="54"/>
+      <c r="G36" s="54"/>
+      <c r="H36" s="45"/>
+      <c r="I36" s="60"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A37" s="78"/>
+      <c r="B37" s="66">
+        <v>17</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D37" s="86" t="s">
+        <v>83</v>
+      </c>
+      <c r="E37" s="52"/>
+      <c r="F37" s="52"/>
+      <c r="G37" s="88" t="s">
+        <v>82</v>
+      </c>
+      <c r="H37" s="55" t="s">
+        <v>78</v>
+      </c>
+      <c r="I37" s="8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A38" s="78"/>
+      <c r="B38" s="71"/>
+      <c r="C38" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="D38" s="87"/>
+      <c r="E38" s="53"/>
+      <c r="F38" s="53"/>
+      <c r="G38" s="89"/>
+      <c r="H38" s="56"/>
+      <c r="I38" s="24" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="78"/>
+      <c r="B39" s="71"/>
+      <c r="C39" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="D39" s="87"/>
+      <c r="E39" s="53"/>
+      <c r="F39" s="53"/>
+      <c r="G39" s="89"/>
+      <c r="H39" s="56"/>
+      <c r="I39" s="46"/>
+    </row>
+    <row r="40" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A40" s="78"/>
+      <c r="B40" s="66">
+        <v>18</v>
+      </c>
+      <c r="C40" s="61" t="s">
+        <v>84</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="E40" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="F40" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="G40" s="52"/>
+      <c r="H40" s="47" t="s">
+        <v>94</v>
+      </c>
+      <c r="I40" s="49" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A41" s="78"/>
+      <c r="B41" s="71"/>
+      <c r="C41" s="62"/>
+      <c r="D41" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="E41" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="F41" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="G41" s="53"/>
+      <c r="H41" s="42" t="s">
         <v>76</v>
       </c>
-      <c r="D36" s="77"/>
-      <c r="E36" s="83"/>
-      <c r="F36" s="48"/>
-      <c r="G36" s="48"/>
-      <c r="H36" s="45"/>
-      <c r="I36" s="73"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37" s="49"/>
-      <c r="B37" s="52">
-        <v>17</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D37" s="61" t="s">
-        <v>84</v>
-      </c>
-      <c r="E37" s="51"/>
-      <c r="F37" s="51"/>
-      <c r="G37" s="63" t="s">
-        <v>83</v>
-      </c>
-      <c r="H37" s="67" t="s">
-        <v>79</v>
-      </c>
-      <c r="I37" s="8" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A38" s="49"/>
-      <c r="B38" s="65"/>
-      <c r="C38" s="19" t="s">
-        <v>115</v>
-      </c>
-      <c r="D38" s="62"/>
-      <c r="E38" s="47"/>
-      <c r="F38" s="47"/>
-      <c r="G38" s="64"/>
-      <c r="H38" s="68"/>
-      <c r="I38" s="24" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="49"/>
-      <c r="B39" s="65"/>
-      <c r="C39" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D39" s="62"/>
-      <c r="E39" s="47"/>
-      <c r="F39" s="47"/>
-      <c r="G39" s="64"/>
-      <c r="H39" s="68"/>
-      <c r="I39" s="46"/>
-    </row>
-    <row r="40" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A40" s="49"/>
-      <c r="B40" s="52">
-        <v>18</v>
-      </c>
-      <c r="C40" s="81" t="s">
-        <v>85</v>
-      </c>
-      <c r="D40" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="E40" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="F40" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="G40" s="51"/>
-      <c r="H40" s="89" t="s">
-        <v>95</v>
-      </c>
-      <c r="I40" s="86" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A41" s="49"/>
-      <c r="B41" s="65"/>
-      <c r="C41" s="82"/>
-      <c r="D41" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="E41" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="F41" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="G41" s="47"/>
-      <c r="H41" s="42" t="s">
-        <v>77</v>
-      </c>
-      <c r="I41" s="87"/>
+      <c r="I41" s="50"/>
     </row>
     <row r="42" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="49"/>
-      <c r="B42" s="53"/>
-      <c r="C42" s="83"/>
+      <c r="A42" s="78"/>
+      <c r="B42" s="67"/>
+      <c r="C42" s="63"/>
       <c r="D42" s="3"/>
       <c r="E42" s="22" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F42" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="G42" s="48"/>
-      <c r="H42" s="90"/>
-      <c r="I42" s="88"/>
+        <v>90</v>
+      </c>
+      <c r="G42" s="54"/>
+      <c r="H42" s="48"/>
+      <c r="I42" s="51"/>
     </row>
     <row r="43" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="49"/>
+      <c r="A43" s="78"/>
       <c r="B43" s="35">
         <v>20</v>
       </c>
@@ -1993,27 +1993,27 @@
       <c r="F43" s="5"/>
       <c r="G43" s="5"/>
       <c r="H43" s="15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I43" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A44" s="50"/>
-      <c r="B44" s="59" t="s">
-        <v>106</v>
-      </c>
-      <c r="C44" s="59"/>
-      <c r="D44" s="59"/>
-      <c r="E44" s="59"/>
-      <c r="F44" s="59"/>
-      <c r="G44" s="59"/>
-      <c r="H44" s="59"/>
-      <c r="I44" s="60"/>
+      <c r="A44" s="79"/>
+      <c r="B44" s="70" t="s">
+        <v>105</v>
+      </c>
+      <c r="C44" s="70"/>
+      <c r="D44" s="70"/>
+      <c r="E44" s="70"/>
+      <c r="F44" s="70"/>
+      <c r="G44" s="70"/>
+      <c r="H44" s="70"/>
+      <c r="I44" s="85"/>
     </row>
     <row r="45" spans="1:9" s="16" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="50"/>
+      <c r="A45" s="79"/>
       <c r="B45" s="18"/>
       <c r="C45" s="17">
         <f t="shared" ref="C45:I45" si="0">COUNTIF(C4:C43, "&lt;&gt;")</f>
@@ -2045,63 +2045,70 @@
       </c>
     </row>
     <row r="46" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="50"/>
-      <c r="B46" s="59" t="str">
+      <c r="A46" s="79"/>
+      <c r="B46" s="70" t="str">
         <f>SUM(C45:I45) &amp; " Total Races (Prior to Breeders' Cup Weekend)"</f>
         <v>98 Total Races (Prior to Breeders' Cup Weekend)</v>
       </c>
-      <c r="C46" s="59"/>
-      <c r="D46" s="59"/>
-      <c r="E46" s="59"/>
-      <c r="F46" s="59"/>
-      <c r="G46" s="59"/>
-      <c r="H46" s="59"/>
-      <c r="I46" s="59"/>
+      <c r="C46" s="70"/>
+      <c r="D46" s="70"/>
+      <c r="E46" s="70"/>
+      <c r="F46" s="70"/>
+      <c r="G46" s="70"/>
+      <c r="H46" s="70"/>
+      <c r="I46" s="70"/>
     </row>
     <row r="47" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="50"/>
-      <c r="B47" s="54" t="s">
+      <c r="A47" s="79"/>
+      <c r="B47" s="80" t="s">
+        <v>103</v>
+      </c>
+      <c r="C47" s="80"/>
+      <c r="D47" s="80"/>
+      <c r="E47" s="81"/>
+      <c r="F47" s="82" t="s">
         <v>104</v>
       </c>
-      <c r="C47" s="54"/>
-      <c r="D47" s="54"/>
-      <c r="E47" s="55"/>
-      <c r="F47" s="56" t="s">
-        <v>105</v>
-      </c>
-      <c r="G47" s="57"/>
-      <c r="H47" s="57"/>
-      <c r="I47" s="58"/>
+      <c r="G47" s="83"/>
+      <c r="H47" s="83"/>
+      <c r="I47" s="84"/>
     </row>
   </sheetData>
   <mergeCells count="79">
-    <mergeCell ref="I40:I42"/>
-    <mergeCell ref="H18:H20"/>
-    <mergeCell ref="G18:G20"/>
-    <mergeCell ref="F18:F20"/>
-    <mergeCell ref="E18:E20"/>
-    <mergeCell ref="H37:H39"/>
-    <mergeCell ref="I30:I31"/>
-    <mergeCell ref="D27:D29"/>
-    <mergeCell ref="I34:I36"/>
-    <mergeCell ref="G34:G36"/>
-    <mergeCell ref="F34:F36"/>
-    <mergeCell ref="E34:E36"/>
-    <mergeCell ref="I21:I23"/>
-    <mergeCell ref="G21:G23"/>
-    <mergeCell ref="E21:E23"/>
-    <mergeCell ref="I15:I17"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="H15:H17"/>
-    <mergeCell ref="I27:I29"/>
-    <mergeCell ref="F27:F29"/>
-    <mergeCell ref="E27:E29"/>
-    <mergeCell ref="I24:I25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="G24:G25"/>
-    <mergeCell ref="H24:H25"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="E4:E6"/>
+    <mergeCell ref="F4:F6"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B47:E47"/>
+    <mergeCell ref="F47:I47"/>
+    <mergeCell ref="B44:I44"/>
+    <mergeCell ref="D37:D39"/>
+    <mergeCell ref="E37:E39"/>
+    <mergeCell ref="F37:F39"/>
+    <mergeCell ref="G37:G39"/>
+    <mergeCell ref="B37:B39"/>
+    <mergeCell ref="C1:I1"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="G15:G17"/>
+    <mergeCell ref="F15:F17"/>
+    <mergeCell ref="A2:A43"/>
+    <mergeCell ref="A44:A47"/>
+    <mergeCell ref="B40:B42"/>
+    <mergeCell ref="C40:C42"/>
+    <mergeCell ref="H4:H6"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="H21:H23"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="G4:G6"/>
+    <mergeCell ref="D34:D36"/>
+    <mergeCell ref="H30:H31"/>
+    <mergeCell ref="E15:E17"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="E11:E13"/>
+    <mergeCell ref="F11:F13"/>
     <mergeCell ref="B46:I46"/>
     <mergeCell ref="G40:G42"/>
     <mergeCell ref="B4:B6"/>
@@ -2118,42 +2125,35 @@
     <mergeCell ref="B18:B20"/>
     <mergeCell ref="D18:D20"/>
     <mergeCell ref="C24:C25"/>
-    <mergeCell ref="B40:B42"/>
-    <mergeCell ref="C40:C42"/>
-    <mergeCell ref="H4:H6"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="H21:H23"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="G4:G6"/>
-    <mergeCell ref="D34:D36"/>
-    <mergeCell ref="H30:H31"/>
-    <mergeCell ref="E15:E17"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="H24:H25"/>
+    <mergeCell ref="I15:I17"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="H15:H17"/>
+    <mergeCell ref="I27:I29"/>
+    <mergeCell ref="F27:F29"/>
+    <mergeCell ref="I24:I25"/>
     <mergeCell ref="I11:I13"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="E11:E13"/>
-    <mergeCell ref="F11:F13"/>
     <mergeCell ref="G11:G13"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="G15:G17"/>
-    <mergeCell ref="F15:F17"/>
-    <mergeCell ref="A2:A43"/>
-    <mergeCell ref="A44:A47"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="E4:E6"/>
-    <mergeCell ref="F4:F6"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B47:E47"/>
-    <mergeCell ref="F47:I47"/>
-    <mergeCell ref="B44:I44"/>
-    <mergeCell ref="D37:D39"/>
-    <mergeCell ref="E37:E39"/>
-    <mergeCell ref="F37:F39"/>
-    <mergeCell ref="G37:G39"/>
-    <mergeCell ref="B37:B39"/>
-    <mergeCell ref="C1:I1"/>
+    <mergeCell ref="D27:D29"/>
+    <mergeCell ref="I34:I36"/>
+    <mergeCell ref="G34:G36"/>
+    <mergeCell ref="F34:F36"/>
+    <mergeCell ref="E34:E36"/>
+    <mergeCell ref="E27:E29"/>
+    <mergeCell ref="I40:I42"/>
+    <mergeCell ref="H18:H20"/>
+    <mergeCell ref="G18:G20"/>
+    <mergeCell ref="F18:F20"/>
+    <mergeCell ref="E18:E20"/>
+    <mergeCell ref="H37:H39"/>
+    <mergeCell ref="I30:I31"/>
+    <mergeCell ref="I21:I23"/>
+    <mergeCell ref="G21:G23"/>
+    <mergeCell ref="E21:E23"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
RTTBC24 Week 13 Results, Week 15 Noms (CD); Draft #5 Stats
</commit_message>
<xml_diff>
--- a/pdf/RTTBC24-Schedule-by-Division.xlsx
+++ b/pdf/RTTBC24-Schedule-by-Division.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/299f8723705ec823/Webmaster/gallop-racing.com/pdf/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1135" documentId="8_{DAECCBE5-FF72-4188-B2F1-1541968A3FDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4C032FCA-238B-4FD9-92CB-168A40812DF3}"/>
+  <xr:revisionPtr revIDLastSave="1141" documentId="8_{DAECCBE5-FF72-4188-B2F1-1541968A3FDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{347618C4-5614-4428-82CB-957CD85D33FE}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{EAD27B02-19FE-4D48-9014-ED6E24DB84F0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{EAD27B02-19FE-4D48-9014-ED6E24DB84F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -194,9 +194,6 @@
     <t>Charles Town Classic S.-G2</t>
   </si>
   <si>
-    <t>Charles Town Oaks S.-G3</t>
-  </si>
-  <si>
     <t>Personal Ensign S.-G1</t>
   </si>
   <si>
@@ -215,9 +212,6 @@
     <t>Pat O'Brien S.-G2</t>
   </si>
   <si>
-    <t>Prioress S.-G2</t>
-  </si>
-  <si>
     <t>Jockey Club Gold Cup-G1</t>
   </si>
   <si>
@@ -245,9 +239,6 @@
     <t>Pocahontas S.-G3</t>
   </si>
   <si>
-    <t>Locust Grove S.-G3</t>
-  </si>
-  <si>
     <t>Cotillion S.-G1</t>
   </si>
   <si>
@@ -384,6 +375,15 @@
   </si>
   <si>
     <t>Test S.-G1</t>
+  </si>
+  <si>
+    <t>Locust Grove S.-G2</t>
+  </si>
+  <si>
+    <t>Prioress S.-G3</t>
+  </si>
+  <si>
+    <t>Charles Town Oaks S.-G2</t>
   </si>
 </sst>
 </file>
@@ -792,8 +792,17 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -804,128 +813,119 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -947,6 +947,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1250,7 +1254,7 @@
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F11" sqref="F11:F13"/>
+      <selection pane="bottomLeft" activeCell="F18" sqref="F18:F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1266,47 +1270,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="47"/>
-      <c r="B1" s="47"/>
-      <c r="C1" s="65" t="s">
-        <v>106</v>
-      </c>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
+      <c r="A1" s="80"/>
+      <c r="B1" s="80"/>
+      <c r="C1" s="91" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="91"/>
+      <c r="G1" s="91"/>
+      <c r="H1" s="91"/>
+      <c r="I1" s="91"/>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="66" t="s">
-        <v>107</v>
+      <c r="A2" s="79" t="s">
+        <v>104</v>
       </c>
       <c r="B2" s="33"/>
       <c r="C2" s="31" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D2" s="31" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E2" s="31" t="s">
+        <v>93</v>
+      </c>
+      <c r="F2" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="G2" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="H2" s="31" t="s">
+        <v>95</v>
+      </c>
+      <c r="I2" s="31" t="s">
         <v>96</v>
       </c>
-      <c r="F2" s="31" t="s">
-        <v>97</v>
-      </c>
-      <c r="G2" s="31" t="s">
-        <v>100</v>
-      </c>
-      <c r="H2" s="31" t="s">
-        <v>98</v>
-      </c>
-      <c r="I2" s="31" t="s">
-        <v>99</v>
-      </c>
     </row>
     <row r="3" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="66"/>
+      <c r="A3" s="79"/>
       <c r="B3" s="34"/>
       <c r="C3" s="32" t="s">
         <v>5</v>
@@ -1331,8 +1335,8 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A4" s="66"/>
-      <c r="B4" s="51">
+      <c r="A4" s="79"/>
+      <c r="B4" s="70">
         <v>1</v>
       </c>
       <c r="C4" s="23" t="s">
@@ -1341,48 +1345,48 @@
       <c r="D4" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="48"/>
-      <c r="F4" s="48"/>
-      <c r="G4" s="73" t="s">
+      <c r="E4" s="51"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="48"/>
+      <c r="H4" s="51"/>
       <c r="I4" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A5" s="66"/>
-      <c r="B5" s="64"/>
+      <c r="A5" s="79"/>
+      <c r="B5" s="73"/>
       <c r="C5" s="10" t="s">
         <v>22</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="74"/>
-      <c r="H5" s="49"/>
+        <v>107</v>
+      </c>
+      <c r="E5" s="52"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="77"/>
+      <c r="H5" s="52"/>
       <c r="I5" s="21" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="66"/>
-      <c r="B6" s="52"/>
+      <c r="A6" s="79"/>
+      <c r="B6" s="71"/>
       <c r="C6" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="3"/>
-      <c r="E6" s="50"/>
-      <c r="F6" s="50"/>
-      <c r="G6" s="75"/>
-      <c r="H6" s="50"/>
+      <c r="E6" s="53"/>
+      <c r="F6" s="53"/>
+      <c r="G6" s="78"/>
+      <c r="H6" s="53"/>
       <c r="I6" s="3"/>
     </row>
     <row r="7" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="66"/>
+      <c r="A7" s="79"/>
       <c r="B7" s="35">
         <v>2</v>
       </c>
@@ -1394,12 +1398,12 @@
         <v>12</v>
       </c>
       <c r="H7" s="15" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="I7" s="4"/>
     </row>
     <row r="8" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="66"/>
+      <c r="A8" s="79"/>
       <c r="B8" s="35">
         <v>3</v>
       </c>
@@ -1416,36 +1420,36 @@
       <c r="I8" s="4"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="66"/>
-      <c r="B9" s="51">
+      <c r="A9" s="79"/>
+      <c r="B9" s="70">
         <v>4</v>
       </c>
-      <c r="C9" s="73" t="s">
+      <c r="C9" s="76" t="s">
         <v>16</v>
       </c>
       <c r="D9" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="48"/>
-      <c r="F9" s="48"/>
-      <c r="G9" s="78"/>
-      <c r="H9" s="76"/>
-      <c r="I9" s="83"/>
+      <c r="E9" s="51"/>
+      <c r="F9" s="51"/>
+      <c r="G9" s="64"/>
+      <c r="H9" s="54"/>
+      <c r="I9" s="66"/>
     </row>
     <row r="10" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="66"/>
-      <c r="B10" s="52"/>
-      <c r="C10" s="75"/>
+      <c r="A10" s="79"/>
+      <c r="B10" s="71"/>
+      <c r="C10" s="78"/>
       <c r="D10" s="12"/>
-      <c r="E10" s="50"/>
-      <c r="F10" s="50"/>
-      <c r="G10" s="79"/>
-      <c r="H10" s="77"/>
-      <c r="I10" s="84"/>
+      <c r="E10" s="53"/>
+      <c r="F10" s="53"/>
+      <c r="G10" s="69"/>
+      <c r="H10" s="68"/>
+      <c r="I10" s="67"/>
     </row>
     <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="66"/>
-      <c r="B11" s="51">
+      <c r="A11" s="79"/>
+      <c r="B11" s="70">
         <v>5</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -1454,52 +1458,52 @@
       <c r="D11" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="48"/>
-      <c r="F11" s="48"/>
-      <c r="G11" s="78" t="s">
+      <c r="E11" s="51"/>
+      <c r="F11" s="51"/>
+      <c r="G11" s="64" t="s">
         <v>18</v>
       </c>
       <c r="H11" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="I11" s="76" t="s">
+      <c r="I11" s="54" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="66"/>
-      <c r="B12" s="64"/>
+      <c r="A12" s="79"/>
+      <c r="B12" s="73"/>
       <c r="C12" s="10" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="49"/>
-      <c r="F12" s="49"/>
-      <c r="G12" s="82"/>
+      <c r="E12" s="52"/>
+      <c r="F12" s="52"/>
+      <c r="G12" s="65"/>
       <c r="H12" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="I12" s="85"/>
+      <c r="I12" s="55"/>
     </row>
     <row r="13" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="66"/>
-      <c r="B13" s="64"/>
+      <c r="A13" s="79"/>
+      <c r="B13" s="73"/>
       <c r="C13" s="7" t="s">
         <v>26</v>
       </c>
       <c r="D13" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E13" s="49"/>
-      <c r="F13" s="49"/>
-      <c r="G13" s="82"/>
+      <c r="E13" s="52"/>
+      <c r="F13" s="52"/>
+      <c r="G13" s="65"/>
       <c r="H13" s="39"/>
-      <c r="I13" s="85"/>
+      <c r="I13" s="55"/>
     </row>
     <row r="14" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="66"/>
+      <c r="A14" s="79"/>
       <c r="B14" s="35">
         <v>6</v>
       </c>
@@ -1514,8 +1518,8 @@
       <c r="I14" s="4"/>
     </row>
     <row r="15" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A15" s="66"/>
-      <c r="B15" s="51">
+      <c r="A15" s="79"/>
+      <c r="B15" s="70">
         <v>7</v>
       </c>
       <c r="C15" s="9" t="s">
@@ -1524,170 +1528,170 @@
       <c r="D15" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="48"/>
-      <c r="F15" s="48"/>
-      <c r="G15" s="48"/>
-      <c r="H15" s="76" t="s">
+      <c r="E15" s="51"/>
+      <c r="F15" s="51"/>
+      <c r="G15" s="51"/>
+      <c r="H15" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="I15" s="48"/>
+      <c r="I15" s="51"/>
     </row>
     <row r="16" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A16" s="66"/>
-      <c r="B16" s="64"/>
+      <c r="A16" s="79"/>
+      <c r="B16" s="73"/>
       <c r="C16" s="19" t="s">
         <v>31</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E16" s="49"/>
-      <c r="F16" s="49"/>
-      <c r="G16" s="49"/>
-      <c r="H16" s="85"/>
-      <c r="I16" s="49"/>
+      <c r="E16" s="52"/>
+      <c r="F16" s="52"/>
+      <c r="G16" s="52"/>
+      <c r="H16" s="55"/>
+      <c r="I16" s="52"/>
     </row>
     <row r="17" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="66"/>
-      <c r="B17" s="52"/>
+      <c r="A17" s="79"/>
+      <c r="B17" s="71"/>
       <c r="C17" s="12" t="s">
         <v>33</v>
       </c>
       <c r="D17" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="E17" s="50"/>
-      <c r="F17" s="50"/>
-      <c r="G17" s="50"/>
-      <c r="H17" s="77"/>
-      <c r="I17" s="50"/>
+      <c r="E17" s="53"/>
+      <c r="F17" s="53"/>
+      <c r="G17" s="53"/>
+      <c r="H17" s="68"/>
+      <c r="I17" s="53"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="66"/>
-      <c r="B18" s="51">
+      <c r="A18" s="79"/>
+      <c r="B18" s="70">
         <v>8</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D18" s="78" t="s">
+      <c r="D18" s="64" t="s">
         <v>40</v>
       </c>
-      <c r="E18" s="48"/>
-      <c r="F18" s="48"/>
-      <c r="G18" s="48"/>
-      <c r="H18" s="48"/>
+      <c r="E18" s="51"/>
+      <c r="F18" s="51"/>
+      <c r="G18" s="51"/>
+      <c r="H18" s="51"/>
       <c r="I18" s="6" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A19" s="66"/>
-      <c r="B19" s="64"/>
+      <c r="A19" s="79"/>
+      <c r="B19" s="73"/>
       <c r="C19" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="D19" s="82"/>
-      <c r="E19" s="49"/>
-      <c r="F19" s="49"/>
-      <c r="G19" s="49"/>
-      <c r="H19" s="49"/>
+      <c r="D19" s="65"/>
+      <c r="E19" s="52"/>
+      <c r="F19" s="52"/>
+      <c r="G19" s="52"/>
+      <c r="H19" s="52"/>
       <c r="I19" s="21" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="66"/>
-      <c r="B20" s="52"/>
+      <c r="A20" s="79"/>
+      <c r="B20" s="71"/>
       <c r="C20" s="3"/>
-      <c r="D20" s="79"/>
-      <c r="E20" s="50"/>
-      <c r="F20" s="50"/>
-      <c r="G20" s="50"/>
-      <c r="H20" s="50"/>
+      <c r="D20" s="69"/>
+      <c r="E20" s="53"/>
+      <c r="F20" s="53"/>
+      <c r="G20" s="53"/>
+      <c r="H20" s="53"/>
       <c r="I20" s="22" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A21" s="66"/>
-      <c r="B21" s="51">
+      <c r="A21" s="79"/>
+      <c r="B21" s="70">
         <v>9</v>
       </c>
       <c r="C21" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="D21" s="73" t="s">
+      <c r="D21" s="76" t="s">
         <v>42</v>
       </c>
-      <c r="E21" s="48"/>
-      <c r="F21" s="78" t="s">
+      <c r="E21" s="51"/>
+      <c r="F21" s="64" t="s">
         <v>45</v>
       </c>
-      <c r="G21" s="48"/>
-      <c r="H21" s="70" t="s">
-        <v>115</v>
-      </c>
-      <c r="I21" s="48"/>
+      <c r="G21" s="51"/>
+      <c r="H21" s="58" t="s">
+        <v>112</v>
+      </c>
+      <c r="I21" s="51"/>
     </row>
     <row r="22" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="66"/>
-      <c r="B22" s="64"/>
+      <c r="A22" s="79"/>
+      <c r="B22" s="73"/>
       <c r="C22" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D22" s="74"/>
-      <c r="E22" s="49"/>
-      <c r="F22" s="82"/>
-      <c r="G22" s="49"/>
-      <c r="H22" s="71"/>
-      <c r="I22" s="49"/>
+      <c r="D22" s="77"/>
+      <c r="E22" s="52"/>
+      <c r="F22" s="65"/>
+      <c r="G22" s="52"/>
+      <c r="H22" s="59"/>
+      <c r="I22" s="52"/>
     </row>
     <row r="23" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="66"/>
-      <c r="B23" s="52"/>
+      <c r="A23" s="79"/>
+      <c r="B23" s="71"/>
       <c r="C23" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="D23" s="75"/>
-      <c r="E23" s="50"/>
-      <c r="F23" s="79"/>
-      <c r="G23" s="50"/>
-      <c r="H23" s="72"/>
-      <c r="I23" s="50"/>
+      <c r="D23" s="78"/>
+      <c r="E23" s="53"/>
+      <c r="F23" s="69"/>
+      <c r="G23" s="53"/>
+      <c r="H23" s="60"/>
+      <c r="I23" s="53"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="66"/>
-      <c r="B24" s="51">
+      <c r="A24" s="79"/>
+      <c r="B24" s="70">
         <v>10</v>
       </c>
-      <c r="C24" s="48"/>
-      <c r="D24" s="48"/>
+      <c r="C24" s="51"/>
+      <c r="D24" s="51"/>
       <c r="E24" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="F24" s="78" t="s">
+      <c r="F24" s="64" t="s">
         <v>47</v>
       </c>
-      <c r="G24" s="48"/>
-      <c r="H24" s="48"/>
-      <c r="I24" s="48"/>
+      <c r="G24" s="51"/>
+      <c r="H24" s="51"/>
+      <c r="I24" s="51"/>
     </row>
     <row r="25" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="66"/>
-      <c r="B25" s="52"/>
-      <c r="C25" s="50"/>
-      <c r="D25" s="50"/>
+      <c r="A25" s="79"/>
+      <c r="B25" s="71"/>
+      <c r="C25" s="53"/>
+      <c r="D25" s="53"/>
       <c r="E25" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="F25" s="79"/>
-      <c r="G25" s="50"/>
-      <c r="H25" s="50"/>
-      <c r="I25" s="50"/>
+      <c r="F25" s="69"/>
+      <c r="G25" s="53"/>
+      <c r="H25" s="53"/>
+      <c r="I25" s="53"/>
     </row>
     <row r="26" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="66"/>
+      <c r="A26" s="79"/>
       <c r="B26" s="41">
         <v>11</v>
       </c>
@@ -1704,291 +1708,291 @@
       <c r="I26" s="2"/>
     </row>
     <row r="27" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A27" s="66"/>
-      <c r="B27" s="51">
+      <c r="A27" s="79"/>
+      <c r="B27" s="70">
         <v>12</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="D27" s="70" t="s">
+      <c r="D27" s="58" t="s">
+        <v>52</v>
+      </c>
+      <c r="E27" s="51"/>
+      <c r="F27" s="61"/>
+      <c r="G27" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="E27" s="48"/>
-      <c r="F27" s="67"/>
-      <c r="G27" s="23" t="s">
+      <c r="H27" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="I27" s="51"/>
+    </row>
+    <row r="28" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A28" s="79"/>
+      <c r="B28" s="73"/>
+      <c r="C28" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="D28" s="59"/>
+      <c r="E28" s="52"/>
+      <c r="F28" s="62"/>
+      <c r="G28" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="H27" s="20" t="s">
+      <c r="H28" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="I27" s="48"/>
-    </row>
-    <row r="28" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A28" s="66"/>
-      <c r="B28" s="64"/>
-      <c r="C28" s="21" t="s">
-        <v>112</v>
-      </c>
-      <c r="D28" s="71"/>
-      <c r="E28" s="49"/>
-      <c r="F28" s="68"/>
-      <c r="G28" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="H28" s="13" t="s">
+      <c r="I28" s="52"/>
+    </row>
+    <row r="29" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="79"/>
+      <c r="B29" s="71"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="60"/>
+      <c r="E29" s="53"/>
+      <c r="F29" s="63"/>
+      <c r="G29" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="I28" s="49"/>
-    </row>
-    <row r="29" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="66"/>
-      <c r="B29" s="52"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="72"/>
-      <c r="E29" s="50"/>
-      <c r="F29" s="69"/>
-      <c r="G29" s="14" t="s">
+      <c r="H29" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="I29" s="53"/>
+    </row>
+    <row r="30" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A30" s="79"/>
+      <c r="B30" s="70">
+        <v>13</v>
+      </c>
+      <c r="C30" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="H29" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="I29" s="50"/>
-    </row>
-    <row r="30" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A30" s="66"/>
-      <c r="B30" s="51">
-        <v>13</v>
-      </c>
-      <c r="C30" s="20" t="s">
+      <c r="D30" s="64" t="s">
         <v>60</v>
       </c>
-      <c r="D30" s="78" t="s">
+      <c r="E30" s="58" t="s">
         <v>62</v>
       </c>
-      <c r="E30" s="70" t="s">
-        <v>64</v>
-      </c>
-      <c r="F30" s="80" t="s">
-        <v>63</v>
-      </c>
-      <c r="G30" s="48"/>
-      <c r="H30" s="76" t="s">
+      <c r="F30" s="74" t="s">
+        <v>61</v>
+      </c>
+      <c r="G30" s="51"/>
+      <c r="H30" s="64" t="s">
+        <v>114</v>
+      </c>
+      <c r="I30" s="51"/>
+    </row>
+    <row r="31" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A31" s="79"/>
+      <c r="B31" s="71"/>
+      <c r="C31" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="I30" s="48"/>
-    </row>
-    <row r="31" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="66"/>
-      <c r="B31" s="52"/>
-      <c r="C31" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="D31" s="79"/>
-      <c r="E31" s="72"/>
-      <c r="F31" s="81"/>
-      <c r="G31" s="50"/>
-      <c r="H31" s="77"/>
-      <c r="I31" s="50"/>
+      <c r="D31" s="69"/>
+      <c r="E31" s="60"/>
+      <c r="F31" s="75"/>
+      <c r="G31" s="53"/>
+      <c r="H31" s="69"/>
+      <c r="I31" s="53"/>
     </row>
     <row r="32" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="66"/>
+      <c r="A32" s="79"/>
       <c r="B32" s="35">
         <v>14</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
       <c r="E32" s="27" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F32" s="28" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G32" s="5"/>
       <c r="H32" s="5"/>
       <c r="I32" s="5"/>
     </row>
     <row r="33" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="66"/>
+      <c r="A33" s="79"/>
       <c r="B33" s="35">
         <v>15</v>
       </c>
       <c r="C33" s="5"/>
-      <c r="D33" s="11" t="s">
-        <v>69</v>
+      <c r="D33" s="15" t="s">
+        <v>113</v>
       </c>
       <c r="E33" s="29" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F33" s="30" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G33" s="5"/>
       <c r="H33" s="5"/>
       <c r="I33" s="5"/>
     </row>
     <row r="34" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A34" s="66"/>
-      <c r="B34" s="51">
+      <c r="A34" s="79"/>
+      <c r="B34" s="70">
         <v>16</v>
       </c>
       <c r="C34" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="D34" s="58" t="s">
+        <v>67</v>
+      </c>
+      <c r="E34" s="61"/>
+      <c r="F34" s="51"/>
+      <c r="G34" s="51"/>
+      <c r="H34" s="38" t="s">
+        <v>70</v>
+      </c>
+      <c r="I34" s="54" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="79"/>
+      <c r="B35" s="73"/>
+      <c r="C35" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="D34" s="70" t="s">
-        <v>70</v>
-      </c>
-      <c r="E34" s="67"/>
-      <c r="F34" s="48"/>
-      <c r="G34" s="48"/>
-      <c r="H34" s="38" t="s">
+      <c r="D35" s="59"/>
+      <c r="E35" s="62"/>
+      <c r="F35" s="52"/>
+      <c r="G35" s="52"/>
+      <c r="H35" s="43" t="s">
+        <v>106</v>
+      </c>
+      <c r="I35" s="55"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36" s="79"/>
+      <c r="B36" s="70">
+        <v>17</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D36" s="87" t="s">
+        <v>80</v>
+      </c>
+      <c r="E36" s="51"/>
+      <c r="F36" s="51"/>
+      <c r="G36" s="89" t="s">
+        <v>79</v>
+      </c>
+      <c r="H36" s="54" t="s">
+        <v>75</v>
+      </c>
+      <c r="I36" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A37" s="79"/>
+      <c r="B37" s="73"/>
+      <c r="C37" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="D37" s="88"/>
+      <c r="E37" s="52"/>
+      <c r="F37" s="52"/>
+      <c r="G37" s="90"/>
+      <c r="H37" s="55"/>
+      <c r="I37" s="56" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="79"/>
+      <c r="B38" s="73"/>
+      <c r="C38" s="47" t="s">
+        <v>72</v>
+      </c>
+      <c r="D38" s="88"/>
+      <c r="E38" s="52"/>
+      <c r="F38" s="52"/>
+      <c r="G38" s="90"/>
+      <c r="H38" s="55"/>
+      <c r="I38" s="56"/>
+    </row>
+    <row r="39" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="79"/>
+      <c r="B39" s="73"/>
+      <c r="C39" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="D39" s="88"/>
+      <c r="E39" s="52"/>
+      <c r="F39" s="52"/>
+      <c r="G39" s="90"/>
+      <c r="H39" s="55"/>
+      <c r="I39" s="57"/>
+    </row>
+    <row r="40" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A40" s="79"/>
+      <c r="B40" s="70">
+        <v>18</v>
+      </c>
+      <c r="C40" s="61" t="s">
+        <v>81</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="E40" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="F40" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="G40" s="51"/>
+      <c r="H40" s="45" t="s">
+        <v>91</v>
+      </c>
+      <c r="I40" s="48" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A41" s="79"/>
+      <c r="B41" s="73"/>
+      <c r="C41" s="62"/>
+      <c r="D41" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="E41" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="F41" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="G41" s="52"/>
+      <c r="H41" s="42" t="s">
         <v>73</v>
       </c>
-      <c r="I34" s="76" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="66"/>
-      <c r="B35" s="64"/>
-      <c r="C35" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="D35" s="71"/>
-      <c r="E35" s="68"/>
-      <c r="F35" s="49"/>
-      <c r="G35" s="49"/>
-      <c r="H35" s="43" t="s">
-        <v>109</v>
-      </c>
-      <c r="I35" s="85"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="66"/>
-      <c r="B36" s="51">
-        <v>17</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="D36" s="60" t="s">
-        <v>83</v>
-      </c>
-      <c r="E36" s="48"/>
-      <c r="F36" s="48"/>
-      <c r="G36" s="62" t="s">
-        <v>82</v>
-      </c>
-      <c r="H36" s="76" t="s">
-        <v>78</v>
-      </c>
-      <c r="I36" s="8" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A37" s="66"/>
-      <c r="B37" s="64"/>
-      <c r="C37" s="19" t="s">
-        <v>114</v>
-      </c>
-      <c r="D37" s="61"/>
-      <c r="E37" s="49"/>
-      <c r="F37" s="49"/>
-      <c r="G37" s="63"/>
-      <c r="H37" s="85"/>
-      <c r="I37" s="90" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="66"/>
-      <c r="B38" s="64"/>
-      <c r="C38" s="89" t="s">
-        <v>75</v>
-      </c>
-      <c r="D38" s="61"/>
-      <c r="E38" s="49"/>
-      <c r="F38" s="49"/>
-      <c r="G38" s="63"/>
-      <c r="H38" s="85"/>
-      <c r="I38" s="90"/>
-    </row>
-    <row r="39" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="66"/>
-      <c r="B39" s="64"/>
-      <c r="C39" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="D39" s="61"/>
-      <c r="E39" s="49"/>
-      <c r="F39" s="49"/>
-      <c r="G39" s="63"/>
-      <c r="H39" s="85"/>
-      <c r="I39" s="91"/>
-    </row>
-    <row r="40" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A40" s="66"/>
-      <c r="B40" s="51">
-        <v>18</v>
-      </c>
-      <c r="C40" s="67" t="s">
-        <v>84</v>
-      </c>
-      <c r="D40" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="E40" s="20" t="s">
-        <v>87</v>
-      </c>
-      <c r="F40" s="20" t="s">
-        <v>85</v>
-      </c>
-      <c r="G40" s="48"/>
-      <c r="H40" s="45" t="s">
-        <v>94</v>
-      </c>
-      <c r="I40" s="86" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A41" s="66"/>
-      <c r="B41" s="64"/>
-      <c r="C41" s="68"/>
-      <c r="D41" s="19" t="s">
-        <v>93</v>
-      </c>
-      <c r="E41" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="F41" s="19" t="s">
-        <v>88</v>
-      </c>
-      <c r="G41" s="49"/>
-      <c r="H41" s="42" t="s">
-        <v>76</v>
-      </c>
-      <c r="I41" s="87"/>
+      <c r="I41" s="49"/>
     </row>
     <row r="42" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="66"/>
-      <c r="B42" s="52"/>
-      <c r="C42" s="69"/>
+      <c r="A42" s="79"/>
+      <c r="B42" s="71"/>
+      <c r="C42" s="63"/>
       <c r="D42" s="3"/>
       <c r="E42" s="22" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F42" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="G42" s="50"/>
+        <v>87</v>
+      </c>
+      <c r="G42" s="53"/>
       <c r="H42" s="46"/>
-      <c r="I42" s="88"/>
+      <c r="I42" s="50"/>
     </row>
     <row r="43" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="66"/>
+      <c r="A43" s="79"/>
       <c r="B43" s="35">
         <v>20</v>
       </c>
@@ -1998,27 +2002,27 @@
       <c r="F43" s="5"/>
       <c r="G43" s="5"/>
       <c r="H43" s="15" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="I43" s="11" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A44" s="47"/>
-      <c r="B44" s="58" t="s">
-        <v>105</v>
-      </c>
-      <c r="C44" s="58"/>
-      <c r="D44" s="58"/>
-      <c r="E44" s="58"/>
-      <c r="F44" s="58"/>
-      <c r="G44" s="58"/>
-      <c r="H44" s="58"/>
-      <c r="I44" s="59"/>
+      <c r="A44" s="80"/>
+      <c r="B44" s="72" t="s">
+        <v>102</v>
+      </c>
+      <c r="C44" s="72"/>
+      <c r="D44" s="72"/>
+      <c r="E44" s="72"/>
+      <c r="F44" s="72"/>
+      <c r="G44" s="72"/>
+      <c r="H44" s="72"/>
+      <c r="I44" s="86"/>
     </row>
     <row r="45" spans="1:9" s="16" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="47"/>
+      <c r="A45" s="80"/>
       <c r="B45" s="18"/>
       <c r="C45" s="17">
         <f t="shared" ref="C45:I45" si="0">COUNTIF(C4:C43, "&lt;&gt;")</f>
@@ -2050,84 +2054,52 @@
       </c>
     </row>
     <row r="46" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="47"/>
-      <c r="B46" s="58" t="str">
+      <c r="A46" s="80"/>
+      <c r="B46" s="72" t="str">
         <f>SUM(C45:I45) &amp; " Total Races (Prior to Breeders' Cup Weekend)"</f>
         <v>98 Total Races (Prior to Breeders' Cup Weekend)</v>
       </c>
-      <c r="C46" s="58"/>
-      <c r="D46" s="58"/>
-      <c r="E46" s="58"/>
-      <c r="F46" s="58"/>
-      <c r="G46" s="58"/>
-      <c r="H46" s="58"/>
-      <c r="I46" s="58"/>
+      <c r="C46" s="72"/>
+      <c r="D46" s="72"/>
+      <c r="E46" s="72"/>
+      <c r="F46" s="72"/>
+      <c r="G46" s="72"/>
+      <c r="H46" s="72"/>
+      <c r="I46" s="72"/>
     </row>
     <row r="47" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="47"/>
-      <c r="B47" s="53" t="s">
-        <v>103</v>
-      </c>
-      <c r="C47" s="53"/>
-      <c r="D47" s="53"/>
-      <c r="E47" s="54"/>
-      <c r="F47" s="55" t="s">
-        <v>104</v>
-      </c>
-      <c r="G47" s="56"/>
-      <c r="H47" s="56"/>
-      <c r="I47" s="57"/>
+      <c r="A47" s="80"/>
+      <c r="B47" s="81" t="s">
+        <v>100</v>
+      </c>
+      <c r="C47" s="81"/>
+      <c r="D47" s="81"/>
+      <c r="E47" s="82"/>
+      <c r="F47" s="83" t="s">
+        <v>101</v>
+      </c>
+      <c r="G47" s="84"/>
+      <c r="H47" s="84"/>
+      <c r="I47" s="85"/>
     </row>
   </sheetData>
   <mergeCells count="80">
-    <mergeCell ref="I40:I42"/>
-    <mergeCell ref="H18:H20"/>
-    <mergeCell ref="G18:G20"/>
-    <mergeCell ref="F18:F20"/>
-    <mergeCell ref="E18:E20"/>
-    <mergeCell ref="H36:H39"/>
-    <mergeCell ref="I30:I31"/>
-    <mergeCell ref="I21:I23"/>
-    <mergeCell ref="G21:G23"/>
-    <mergeCell ref="E21:E23"/>
-    <mergeCell ref="I37:I39"/>
-    <mergeCell ref="D27:D29"/>
-    <mergeCell ref="I34:I35"/>
-    <mergeCell ref="G34:G35"/>
-    <mergeCell ref="F34:F35"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="E27:E29"/>
-    <mergeCell ref="I27:I29"/>
-    <mergeCell ref="F27:F29"/>
-    <mergeCell ref="I24:I25"/>
-    <mergeCell ref="I11:I13"/>
-    <mergeCell ref="G11:G13"/>
-    <mergeCell ref="G24:G25"/>
-    <mergeCell ref="H24:H25"/>
-    <mergeCell ref="I15:I17"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="H15:H17"/>
-    <mergeCell ref="D18:D20"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="E11:E13"/>
-    <mergeCell ref="F11:F13"/>
-    <mergeCell ref="B46:I46"/>
-    <mergeCell ref="G40:G42"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="G30:G31"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="B27:B29"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="F30:F31"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="D21:D23"/>
-    <mergeCell ref="F21:F23"/>
-    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="E4:E6"/>
+    <mergeCell ref="F4:F6"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B47:E47"/>
+    <mergeCell ref="F47:I47"/>
+    <mergeCell ref="B44:I44"/>
+    <mergeCell ref="D36:D39"/>
+    <mergeCell ref="E36:E39"/>
+    <mergeCell ref="F36:F39"/>
+    <mergeCell ref="G36:G39"/>
+    <mergeCell ref="B36:B39"/>
+    <mergeCell ref="C1:I1"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="G15:G17"/>
+    <mergeCell ref="F15:F17"/>
     <mergeCell ref="A2:A43"/>
     <mergeCell ref="A44:A47"/>
     <mergeCell ref="B40:B42"/>
@@ -2144,22 +2116,54 @@
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="G9:G10"/>
     <mergeCell ref="H9:H10"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="E4:E6"/>
-    <mergeCell ref="F4:F6"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B47:E47"/>
-    <mergeCell ref="F47:I47"/>
-    <mergeCell ref="B44:I44"/>
-    <mergeCell ref="D36:D39"/>
-    <mergeCell ref="E36:E39"/>
-    <mergeCell ref="F36:F39"/>
-    <mergeCell ref="G36:G39"/>
-    <mergeCell ref="B36:B39"/>
-    <mergeCell ref="C1:I1"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="G15:G17"/>
-    <mergeCell ref="F15:F17"/>
+    <mergeCell ref="B46:I46"/>
+    <mergeCell ref="G40:G42"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="G30:G31"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="D21:D23"/>
+    <mergeCell ref="F21:F23"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="H15:H17"/>
+    <mergeCell ref="D18:D20"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="E11:E13"/>
+    <mergeCell ref="F11:F13"/>
+    <mergeCell ref="I11:I13"/>
+    <mergeCell ref="G11:G13"/>
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="H24:H25"/>
+    <mergeCell ref="I15:I17"/>
+    <mergeCell ref="D27:D29"/>
+    <mergeCell ref="I34:I35"/>
+    <mergeCell ref="G34:G35"/>
+    <mergeCell ref="F34:F35"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="E27:E29"/>
+    <mergeCell ref="I27:I29"/>
+    <mergeCell ref="F27:F29"/>
+    <mergeCell ref="I40:I42"/>
+    <mergeCell ref="H18:H20"/>
+    <mergeCell ref="G18:G20"/>
+    <mergeCell ref="F18:F20"/>
+    <mergeCell ref="E18:E20"/>
+    <mergeCell ref="H36:H39"/>
+    <mergeCell ref="I30:I31"/>
+    <mergeCell ref="I21:I23"/>
+    <mergeCell ref="G21:G23"/>
+    <mergeCell ref="E21:E23"/>
+    <mergeCell ref="I37:I39"/>
+    <mergeCell ref="I24:I25"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
GRCW-804; Week 17 Entries (RP, BAQ); Week 18 Noms (BAQ, SA); GRCW-805; Draft #6 Opens
</commit_message>
<xml_diff>
--- a/pdf/RTTBC24-Schedule-by-Division.xlsx
+++ b/pdf/RTTBC24-Schedule-by-Division.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/299f8723705ec823/Webmaster/gallop-racing.com/pdf/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1141" documentId="8_{DAECCBE5-FF72-4188-B2F1-1541968A3FDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{347618C4-5614-4428-82CB-957CD85D33FE}"/>
+  <xr:revisionPtr revIDLastSave="1142" documentId="8_{DAECCBE5-FF72-4188-B2F1-1541968A3FDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{06D003ED-C125-486A-8E7F-AA7C63C97A38}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{EAD27B02-19FE-4D48-9014-ED6E24DB84F0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{EAD27B02-19FE-4D48-9014-ED6E24DB84F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -299,9 +299,6 @@
     <t>American Pharoah S.-G1</t>
   </si>
   <si>
-    <t>Chandelier S.-G2</t>
-  </si>
-  <si>
     <t>Claiborne Breed. Fut.-G1</t>
   </si>
   <si>
@@ -384,6 +381,9 @@
   </si>
   <si>
     <t>Charles Town Oaks S.-G2</t>
+  </si>
+  <si>
+    <t>Oak Leaf S.-G2</t>
   </si>
 </sst>
 </file>
@@ -795,6 +795,123 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -802,21 +919,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -824,108 +926,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1253,8 +1253,8 @@
   <dimension ref="A1:I47"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F18" sqref="F18:F20"/>
+      <pane ySplit="3" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1270,47 +1270,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="80"/>
-      <c r="B1" s="80"/>
-      <c r="C1" s="91" t="s">
+      <c r="A1" s="48"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="66" t="s">
+        <v>102</v>
+      </c>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+    </row>
+    <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A2" s="67" t="s">
         <v>103</v>
-      </c>
-      <c r="D1" s="91"/>
-      <c r="E1" s="91"/>
-      <c r="F1" s="91"/>
-      <c r="G1" s="91"/>
-      <c r="H1" s="91"/>
-      <c r="I1" s="91"/>
-    </row>
-    <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="79" t="s">
-        <v>104</v>
       </c>
       <c r="B2" s="33"/>
       <c r="C2" s="31" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D2" s="31" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E2" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="F2" s="31" t="s">
         <v>93</v>
       </c>
-      <c r="F2" s="31" t="s">
+      <c r="G2" s="31" t="s">
+        <v>96</v>
+      </c>
+      <c r="H2" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="G2" s="31" t="s">
-        <v>97</v>
-      </c>
-      <c r="H2" s="31" t="s">
+      <c r="I2" s="31" t="s">
         <v>95</v>
       </c>
-      <c r="I2" s="31" t="s">
-        <v>96</v>
-      </c>
     </row>
     <row r="3" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="79"/>
+      <c r="A3" s="67"/>
       <c r="B3" s="34"/>
       <c r="C3" s="32" t="s">
         <v>5</v>
@@ -1335,8 +1335,8 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A4" s="79"/>
-      <c r="B4" s="70">
+      <c r="A4" s="67"/>
+      <c r="B4" s="52">
         <v>1</v>
       </c>
       <c r="C4" s="23" t="s">
@@ -1345,48 +1345,48 @@
       <c r="D4" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="51"/>
-      <c r="F4" s="51"/>
-      <c r="G4" s="76" t="s">
+      <c r="E4" s="49"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="74" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="51"/>
+      <c r="H4" s="49"/>
       <c r="I4" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A5" s="79"/>
-      <c r="B5" s="73"/>
+      <c r="A5" s="67"/>
+      <c r="B5" s="65"/>
       <c r="C5" s="10" t="s">
         <v>22</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="E5" s="52"/>
-      <c r="F5" s="52"/>
-      <c r="G5" s="77"/>
-      <c r="H5" s="52"/>
+        <v>106</v>
+      </c>
+      <c r="E5" s="50"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="75"/>
+      <c r="H5" s="50"/>
       <c r="I5" s="21" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="79"/>
-      <c r="B6" s="71"/>
+      <c r="A6" s="67"/>
+      <c r="B6" s="53"/>
       <c r="C6" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="3"/>
-      <c r="E6" s="53"/>
-      <c r="F6" s="53"/>
-      <c r="G6" s="78"/>
-      <c r="H6" s="53"/>
+      <c r="E6" s="51"/>
+      <c r="F6" s="51"/>
+      <c r="G6" s="76"/>
+      <c r="H6" s="51"/>
       <c r="I6" s="3"/>
     </row>
     <row r="7" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="79"/>
+      <c r="A7" s="67"/>
       <c r="B7" s="35">
         <v>2</v>
       </c>
@@ -1398,12 +1398,12 @@
         <v>12</v>
       </c>
       <c r="H7" s="15" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I7" s="4"/>
     </row>
     <row r="8" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="79"/>
+      <c r="A8" s="67"/>
       <c r="B8" s="35">
         <v>3</v>
       </c>
@@ -1420,36 +1420,36 @@
       <c r="I8" s="4"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="79"/>
-      <c r="B9" s="70">
+      <c r="A9" s="67"/>
+      <c r="B9" s="52">
         <v>4</v>
       </c>
-      <c r="C9" s="76" t="s">
+      <c r="C9" s="74" t="s">
         <v>16</v>
       </c>
       <c r="D9" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="51"/>
-      <c r="F9" s="51"/>
-      <c r="G9" s="64"/>
-      <c r="H9" s="54"/>
-      <c r="I9" s="66"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="49"/>
+      <c r="G9" s="77"/>
+      <c r="H9" s="79"/>
+      <c r="I9" s="84"/>
     </row>
     <row r="10" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="79"/>
-      <c r="B10" s="71"/>
-      <c r="C10" s="78"/>
+      <c r="A10" s="67"/>
+      <c r="B10" s="53"/>
+      <c r="C10" s="76"/>
       <c r="D10" s="12"/>
-      <c r="E10" s="53"/>
-      <c r="F10" s="53"/>
-      <c r="G10" s="69"/>
-      <c r="H10" s="68"/>
-      <c r="I10" s="67"/>
+      <c r="E10" s="51"/>
+      <c r="F10" s="51"/>
+      <c r="G10" s="78"/>
+      <c r="H10" s="80"/>
+      <c r="I10" s="85"/>
     </row>
     <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="79"/>
-      <c r="B11" s="70">
+      <c r="A11" s="67"/>
+      <c r="B11" s="52">
         <v>5</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -1458,52 +1458,52 @@
       <c r="D11" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="51"/>
-      <c r="F11" s="51"/>
-      <c r="G11" s="64" t="s">
+      <c r="E11" s="49"/>
+      <c r="F11" s="49"/>
+      <c r="G11" s="77" t="s">
         <v>18</v>
       </c>
       <c r="H11" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="I11" s="54" t="s">
+      <c r="I11" s="79" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="79"/>
-      <c r="B12" s="73"/>
+      <c r="A12" s="67"/>
+      <c r="B12" s="65"/>
       <c r="C12" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="52"/>
-      <c r="F12" s="52"/>
-      <c r="G12" s="65"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="83"/>
       <c r="H12" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="I12" s="55"/>
+      <c r="I12" s="86"/>
     </row>
     <row r="13" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="79"/>
-      <c r="B13" s="73"/>
+      <c r="A13" s="67"/>
+      <c r="B13" s="65"/>
       <c r="C13" s="7" t="s">
         <v>26</v>
       </c>
       <c r="D13" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E13" s="52"/>
-      <c r="F13" s="52"/>
-      <c r="G13" s="65"/>
+      <c r="E13" s="50"/>
+      <c r="F13" s="50"/>
+      <c r="G13" s="83"/>
       <c r="H13" s="39"/>
-      <c r="I13" s="55"/>
+      <c r="I13" s="86"/>
     </row>
     <row r="14" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="79"/>
+      <c r="A14" s="67"/>
       <c r="B14" s="35">
         <v>6</v>
       </c>
@@ -1518,8 +1518,8 @@
       <c r="I14" s="4"/>
     </row>
     <row r="15" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A15" s="79"/>
-      <c r="B15" s="70">
+      <c r="A15" s="67"/>
+      <c r="B15" s="52">
         <v>7</v>
       </c>
       <c r="C15" s="9" t="s">
@@ -1528,170 +1528,170 @@
       <c r="D15" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="51"/>
-      <c r="F15" s="51"/>
-      <c r="G15" s="51"/>
-      <c r="H15" s="54" t="s">
+      <c r="E15" s="49"/>
+      <c r="F15" s="49"/>
+      <c r="G15" s="49"/>
+      <c r="H15" s="79" t="s">
         <v>34</v>
       </c>
-      <c r="I15" s="51"/>
+      <c r="I15" s="49"/>
     </row>
     <row r="16" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A16" s="79"/>
-      <c r="B16" s="73"/>
+      <c r="A16" s="67"/>
+      <c r="B16" s="65"/>
       <c r="C16" s="19" t="s">
         <v>31</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E16" s="52"/>
-      <c r="F16" s="52"/>
-      <c r="G16" s="52"/>
-      <c r="H16" s="55"/>
-      <c r="I16" s="52"/>
+      <c r="E16" s="50"/>
+      <c r="F16" s="50"/>
+      <c r="G16" s="50"/>
+      <c r="H16" s="86"/>
+      <c r="I16" s="50"/>
     </row>
     <row r="17" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="79"/>
-      <c r="B17" s="71"/>
+      <c r="A17" s="67"/>
+      <c r="B17" s="53"/>
       <c r="C17" s="12" t="s">
         <v>33</v>
       </c>
       <c r="D17" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="E17" s="53"/>
-      <c r="F17" s="53"/>
-      <c r="G17" s="53"/>
-      <c r="H17" s="68"/>
-      <c r="I17" s="53"/>
+      <c r="E17" s="51"/>
+      <c r="F17" s="51"/>
+      <c r="G17" s="51"/>
+      <c r="H17" s="80"/>
+      <c r="I17" s="51"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="79"/>
-      <c r="B18" s="70">
+      <c r="A18" s="67"/>
+      <c r="B18" s="52">
         <v>8</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D18" s="64" t="s">
+      <c r="D18" s="77" t="s">
         <v>40</v>
       </c>
-      <c r="E18" s="51"/>
-      <c r="F18" s="51"/>
-      <c r="G18" s="51"/>
-      <c r="H18" s="51"/>
+      <c r="E18" s="49"/>
+      <c r="F18" s="49"/>
+      <c r="G18" s="49"/>
+      <c r="H18" s="49"/>
       <c r="I18" s="6" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A19" s="79"/>
-      <c r="B19" s="73"/>
+      <c r="A19" s="67"/>
+      <c r="B19" s="65"/>
       <c r="C19" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="D19" s="65"/>
-      <c r="E19" s="52"/>
-      <c r="F19" s="52"/>
-      <c r="G19" s="52"/>
-      <c r="H19" s="52"/>
+      <c r="D19" s="83"/>
+      <c r="E19" s="50"/>
+      <c r="F19" s="50"/>
+      <c r="G19" s="50"/>
+      <c r="H19" s="50"/>
       <c r="I19" s="21" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="79"/>
-      <c r="B20" s="71"/>
+      <c r="A20" s="67"/>
+      <c r="B20" s="53"/>
       <c r="C20" s="3"/>
-      <c r="D20" s="69"/>
-      <c r="E20" s="53"/>
-      <c r="F20" s="53"/>
-      <c r="G20" s="53"/>
-      <c r="H20" s="53"/>
+      <c r="D20" s="78"/>
+      <c r="E20" s="51"/>
+      <c r="F20" s="51"/>
+      <c r="G20" s="51"/>
+      <c r="H20" s="51"/>
       <c r="I20" s="22" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A21" s="79"/>
-      <c r="B21" s="70">
+      <c r="A21" s="67"/>
+      <c r="B21" s="52">
         <v>9</v>
       </c>
       <c r="C21" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="D21" s="76" t="s">
+      <c r="D21" s="74" t="s">
         <v>42</v>
       </c>
-      <c r="E21" s="51"/>
-      <c r="F21" s="64" t="s">
+      <c r="E21" s="49"/>
+      <c r="F21" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="G21" s="51"/>
-      <c r="H21" s="58" t="s">
-        <v>112</v>
-      </c>
-      <c r="I21" s="51"/>
+      <c r="G21" s="49"/>
+      <c r="H21" s="71" t="s">
+        <v>111</v>
+      </c>
+      <c r="I21" s="49"/>
     </row>
     <row r="22" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="79"/>
-      <c r="B22" s="73"/>
+      <c r="A22" s="67"/>
+      <c r="B22" s="65"/>
       <c r="C22" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D22" s="77"/>
-      <c r="E22" s="52"/>
-      <c r="F22" s="65"/>
-      <c r="G22" s="52"/>
-      <c r="H22" s="59"/>
-      <c r="I22" s="52"/>
+      <c r="D22" s="75"/>
+      <c r="E22" s="50"/>
+      <c r="F22" s="83"/>
+      <c r="G22" s="50"/>
+      <c r="H22" s="72"/>
+      <c r="I22" s="50"/>
     </row>
     <row r="23" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="79"/>
-      <c r="B23" s="71"/>
+      <c r="A23" s="67"/>
+      <c r="B23" s="53"/>
       <c r="C23" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="D23" s="78"/>
-      <c r="E23" s="53"/>
-      <c r="F23" s="69"/>
-      <c r="G23" s="53"/>
-      <c r="H23" s="60"/>
-      <c r="I23" s="53"/>
+      <c r="D23" s="76"/>
+      <c r="E23" s="51"/>
+      <c r="F23" s="78"/>
+      <c r="G23" s="51"/>
+      <c r="H23" s="73"/>
+      <c r="I23" s="51"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="79"/>
-      <c r="B24" s="70">
+      <c r="A24" s="67"/>
+      <c r="B24" s="52">
         <v>10</v>
       </c>
-      <c r="C24" s="51"/>
-      <c r="D24" s="51"/>
+      <c r="C24" s="49"/>
+      <c r="D24" s="49"/>
       <c r="E24" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="F24" s="64" t="s">
+      <c r="F24" s="77" t="s">
         <v>47</v>
       </c>
-      <c r="G24" s="51"/>
-      <c r="H24" s="51"/>
-      <c r="I24" s="51"/>
+      <c r="G24" s="49"/>
+      <c r="H24" s="49"/>
+      <c r="I24" s="49"/>
     </row>
     <row r="25" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="79"/>
-      <c r="B25" s="71"/>
-      <c r="C25" s="53"/>
-      <c r="D25" s="53"/>
+      <c r="A25" s="67"/>
+      <c r="B25" s="53"/>
+      <c r="C25" s="51"/>
+      <c r="D25" s="51"/>
       <c r="E25" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="F25" s="69"/>
-      <c r="G25" s="53"/>
-      <c r="H25" s="53"/>
-      <c r="I25" s="53"/>
+      <c r="F25" s="78"/>
+      <c r="G25" s="51"/>
+      <c r="H25" s="51"/>
+      <c r="I25" s="51"/>
     </row>
     <row r="26" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="79"/>
+      <c r="A26" s="67"/>
       <c r="B26" s="41">
         <v>11</v>
       </c>
@@ -1708,96 +1708,96 @@
       <c r="I26" s="2"/>
     </row>
     <row r="27" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A27" s="79"/>
-      <c r="B27" s="70">
+      <c r="A27" s="67"/>
+      <c r="B27" s="52">
         <v>12</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="D27" s="58" t="s">
+      <c r="D27" s="71" t="s">
         <v>52</v>
       </c>
-      <c r="E27" s="51"/>
-      <c r="F27" s="61"/>
+      <c r="E27" s="49"/>
+      <c r="F27" s="68"/>
       <c r="G27" s="23" t="s">
         <v>53</v>
       </c>
       <c r="H27" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="I27" s="51"/>
+      <c r="I27" s="49"/>
     </row>
     <row r="28" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A28" s="79"/>
-      <c r="B28" s="73"/>
+      <c r="A28" s="67"/>
+      <c r="B28" s="65"/>
       <c r="C28" s="21" t="s">
-        <v>109</v>
-      </c>
-      <c r="D28" s="59"/>
-      <c r="E28" s="52"/>
-      <c r="F28" s="62"/>
+        <v>108</v>
+      </c>
+      <c r="D28" s="72"/>
+      <c r="E28" s="50"/>
+      <c r="F28" s="69"/>
       <c r="G28" s="21" t="s">
         <v>54</v>
       </c>
       <c r="H28" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="I28" s="52"/>
+      <c r="I28" s="50"/>
     </row>
     <row r="29" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="79"/>
-      <c r="B29" s="71"/>
+      <c r="A29" s="67"/>
+      <c r="B29" s="53"/>
       <c r="C29" s="3"/>
-      <c r="D29" s="60"/>
-      <c r="E29" s="53"/>
-      <c r="F29" s="63"/>
+      <c r="D29" s="73"/>
+      <c r="E29" s="51"/>
+      <c r="F29" s="70"/>
       <c r="G29" s="14" t="s">
         <v>57</v>
       </c>
       <c r="H29" s="26" t="s">
-        <v>115</v>
-      </c>
-      <c r="I29" s="53"/>
+        <v>114</v>
+      </c>
+      <c r="I29" s="51"/>
     </row>
     <row r="30" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A30" s="79"/>
-      <c r="B30" s="70">
+      <c r="A30" s="67"/>
+      <c r="B30" s="52">
         <v>13</v>
       </c>
       <c r="C30" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="D30" s="64" t="s">
+      <c r="D30" s="77" t="s">
         <v>60</v>
       </c>
-      <c r="E30" s="58" t="s">
+      <c r="E30" s="71" t="s">
         <v>62</v>
       </c>
-      <c r="F30" s="74" t="s">
+      <c r="F30" s="81" t="s">
         <v>61</v>
       </c>
-      <c r="G30" s="51"/>
-      <c r="H30" s="64" t="s">
-        <v>114</v>
-      </c>
-      <c r="I30" s="51"/>
+      <c r="G30" s="49"/>
+      <c r="H30" s="77" t="s">
+        <v>113</v>
+      </c>
+      <c r="I30" s="49"/>
     </row>
     <row r="31" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="79"/>
-      <c r="B31" s="71"/>
+      <c r="A31" s="67"/>
+      <c r="B31" s="53"/>
       <c r="C31" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="D31" s="69"/>
-      <c r="E31" s="60"/>
-      <c r="F31" s="75"/>
-      <c r="G31" s="53"/>
-      <c r="H31" s="69"/>
-      <c r="I31" s="53"/>
+      <c r="D31" s="78"/>
+      <c r="E31" s="73"/>
+      <c r="F31" s="82"/>
+      <c r="G31" s="51"/>
+      <c r="H31" s="78"/>
+      <c r="I31" s="51"/>
     </row>
     <row r="32" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="79"/>
+      <c r="A32" s="67"/>
       <c r="B32" s="35">
         <v>14</v>
       </c>
@@ -1814,13 +1814,13 @@
       <c r="I32" s="5"/>
     </row>
     <row r="33" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="79"/>
+      <c r="A33" s="67"/>
       <c r="B33" s="35">
         <v>15</v>
       </c>
       <c r="C33" s="5"/>
       <c r="D33" s="15" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E33" s="29" t="s">
         <v>65</v>
@@ -1833,58 +1833,58 @@
       <c r="I33" s="5"/>
     </row>
     <row r="34" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A34" s="79"/>
-      <c r="B34" s="70">
+      <c r="A34" s="67"/>
+      <c r="B34" s="52">
         <v>16</v>
       </c>
       <c r="C34" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="D34" s="58" t="s">
+      <c r="D34" s="71" t="s">
         <v>67</v>
       </c>
-      <c r="E34" s="61"/>
-      <c r="F34" s="51"/>
-      <c r="G34" s="51"/>
+      <c r="E34" s="68"/>
+      <c r="F34" s="49"/>
+      <c r="G34" s="49"/>
       <c r="H34" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="I34" s="54" t="s">
+      <c r="I34" s="79" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="79"/>
-      <c r="B35" s="73"/>
+      <c r="A35" s="67"/>
+      <c r="B35" s="65"/>
       <c r="C35" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="D35" s="59"/>
-      <c r="E35" s="62"/>
-      <c r="F35" s="52"/>
-      <c r="G35" s="52"/>
+      <c r="D35" s="72"/>
+      <c r="E35" s="69"/>
+      <c r="F35" s="50"/>
+      <c r="G35" s="50"/>
       <c r="H35" s="43" t="s">
-        <v>106</v>
-      </c>
-      <c r="I35" s="55"/>
+        <v>105</v>
+      </c>
+      <c r="I35" s="86"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="79"/>
-      <c r="B36" s="70">
+      <c r="A36" s="67"/>
+      <c r="B36" s="52">
         <v>17</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="D36" s="87" t="s">
+      <c r="D36" s="61" t="s">
         <v>80</v>
       </c>
-      <c r="E36" s="51"/>
-      <c r="F36" s="51"/>
-      <c r="G36" s="89" t="s">
+      <c r="E36" s="49"/>
+      <c r="F36" s="49"/>
+      <c r="G36" s="63" t="s">
         <v>79</v>
       </c>
-      <c r="H36" s="54" t="s">
+      <c r="H36" s="79" t="s">
         <v>75</v>
       </c>
       <c r="I36" s="8" t="s">
@@ -1892,56 +1892,56 @@
       </c>
     </row>
     <row r="37" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A37" s="79"/>
-      <c r="B37" s="73"/>
+      <c r="A37" s="67"/>
+      <c r="B37" s="65"/>
       <c r="C37" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="D37" s="88"/>
-      <c r="E37" s="52"/>
-      <c r="F37" s="52"/>
-      <c r="G37" s="90"/>
-      <c r="H37" s="55"/>
-      <c r="I37" s="56" t="s">
+        <v>110</v>
+      </c>
+      <c r="D37" s="62"/>
+      <c r="E37" s="50"/>
+      <c r="F37" s="50"/>
+      <c r="G37" s="64"/>
+      <c r="H37" s="86"/>
+      <c r="I37" s="90" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="79"/>
-      <c r="B38" s="73"/>
+      <c r="A38" s="67"/>
+      <c r="B38" s="65"/>
       <c r="C38" s="47" t="s">
         <v>72</v>
       </c>
-      <c r="D38" s="88"/>
-      <c r="E38" s="52"/>
-      <c r="F38" s="52"/>
-      <c r="G38" s="90"/>
-      <c r="H38" s="55"/>
-      <c r="I38" s="56"/>
+      <c r="D38" s="62"/>
+      <c r="E38" s="50"/>
+      <c r="F38" s="50"/>
+      <c r="G38" s="64"/>
+      <c r="H38" s="86"/>
+      <c r="I38" s="90"/>
     </row>
     <row r="39" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="79"/>
-      <c r="B39" s="73"/>
+      <c r="A39" s="67"/>
+      <c r="B39" s="65"/>
       <c r="C39" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="D39" s="88"/>
-      <c r="E39" s="52"/>
-      <c r="F39" s="52"/>
-      <c r="G39" s="90"/>
-      <c r="H39" s="55"/>
-      <c r="I39" s="57"/>
+      <c r="D39" s="62"/>
+      <c r="E39" s="50"/>
+      <c r="F39" s="50"/>
+      <c r="G39" s="64"/>
+      <c r="H39" s="86"/>
+      <c r="I39" s="91"/>
     </row>
     <row r="40" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A40" s="79"/>
-      <c r="B40" s="70">
+      <c r="A40" s="67"/>
+      <c r="B40" s="52">
         <v>18</v>
       </c>
-      <c r="C40" s="61" t="s">
+      <c r="C40" s="68" t="s">
         <v>81</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E40" s="20" t="s">
         <v>84</v>
@@ -1949,20 +1949,20 @@
       <c r="F40" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="G40" s="51"/>
+      <c r="G40" s="49"/>
       <c r="H40" s="45" t="s">
-        <v>91</v>
-      </c>
-      <c r="I40" s="48" t="s">
+        <v>90</v>
+      </c>
+      <c r="I40" s="87" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A41" s="79"/>
-      <c r="B41" s="73"/>
-      <c r="C41" s="62"/>
+      <c r="A41" s="67"/>
+      <c r="B41" s="65"/>
+      <c r="C41" s="69"/>
       <c r="D41" s="19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E41" s="19" t="s">
         <v>86</v>
@@ -1970,29 +1970,29 @@
       <c r="F41" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="G41" s="52"/>
+      <c r="G41" s="50"/>
       <c r="H41" s="42" t="s">
         <v>73</v>
       </c>
-      <c r="I41" s="49"/>
+      <c r="I41" s="88"/>
     </row>
     <row r="42" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="79"/>
-      <c r="B42" s="71"/>
-      <c r="C42" s="63"/>
+      <c r="A42" s="67"/>
+      <c r="B42" s="53"/>
+      <c r="C42" s="70"/>
       <c r="D42" s="3"/>
       <c r="E42" s="22" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F42" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="G42" s="53"/>
+        <v>115</v>
+      </c>
+      <c r="G42" s="51"/>
       <c r="H42" s="46"/>
-      <c r="I42" s="50"/>
+      <c r="I42" s="89"/>
     </row>
     <row r="43" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="79"/>
+      <c r="A43" s="67"/>
       <c r="B43" s="35">
         <v>20</v>
       </c>
@@ -2002,27 +2002,27 @@
       <c r="F43" s="5"/>
       <c r="G43" s="5"/>
       <c r="H43" s="15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I43" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A44" s="80"/>
-      <c r="B44" s="72" t="s">
-        <v>102</v>
-      </c>
-      <c r="C44" s="72"/>
-      <c r="D44" s="72"/>
-      <c r="E44" s="72"/>
-      <c r="F44" s="72"/>
-      <c r="G44" s="72"/>
-      <c r="H44" s="72"/>
-      <c r="I44" s="86"/>
+      <c r="A44" s="48"/>
+      <c r="B44" s="59" t="s">
+        <v>101</v>
+      </c>
+      <c r="C44" s="59"/>
+      <c r="D44" s="59"/>
+      <c r="E44" s="59"/>
+      <c r="F44" s="59"/>
+      <c r="G44" s="59"/>
+      <c r="H44" s="59"/>
+      <c r="I44" s="60"/>
     </row>
     <row r="45" spans="1:9" s="16" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="80"/>
+      <c r="A45" s="48"/>
       <c r="B45" s="18"/>
       <c r="C45" s="17">
         <f t="shared" ref="C45:I45" si="0">COUNTIF(C4:C43, "&lt;&gt;")</f>
@@ -2054,36 +2054,100 @@
       </c>
     </row>
     <row r="46" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="80"/>
-      <c r="B46" s="72" t="str">
+      <c r="A46" s="48"/>
+      <c r="B46" s="59" t="str">
         <f>SUM(C45:I45) &amp; " Total Races (Prior to Breeders' Cup Weekend)"</f>
         <v>98 Total Races (Prior to Breeders' Cup Weekend)</v>
       </c>
-      <c r="C46" s="72"/>
-      <c r="D46" s="72"/>
-      <c r="E46" s="72"/>
-      <c r="F46" s="72"/>
-      <c r="G46" s="72"/>
-      <c r="H46" s="72"/>
-      <c r="I46" s="72"/>
+      <c r="C46" s="59"/>
+      <c r="D46" s="59"/>
+      <c r="E46" s="59"/>
+      <c r="F46" s="59"/>
+      <c r="G46" s="59"/>
+      <c r="H46" s="59"/>
+      <c r="I46" s="59"/>
     </row>
     <row r="47" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="80"/>
-      <c r="B47" s="81" t="s">
+      <c r="A47" s="48"/>
+      <c r="B47" s="54" t="s">
+        <v>99</v>
+      </c>
+      <c r="C47" s="54"/>
+      <c r="D47" s="54"/>
+      <c r="E47" s="55"/>
+      <c r="F47" s="56" t="s">
         <v>100</v>
       </c>
-      <c r="C47" s="81"/>
-      <c r="D47" s="81"/>
-      <c r="E47" s="82"/>
-      <c r="F47" s="83" t="s">
-        <v>101</v>
-      </c>
-      <c r="G47" s="84"/>
-      <c r="H47" s="84"/>
-      <c r="I47" s="85"/>
+      <c r="G47" s="57"/>
+      <c r="H47" s="57"/>
+      <c r="I47" s="58"/>
     </row>
   </sheetData>
   <mergeCells count="80">
+    <mergeCell ref="I40:I42"/>
+    <mergeCell ref="H18:H20"/>
+    <mergeCell ref="G18:G20"/>
+    <mergeCell ref="F18:F20"/>
+    <mergeCell ref="E18:E20"/>
+    <mergeCell ref="H36:H39"/>
+    <mergeCell ref="I30:I31"/>
+    <mergeCell ref="I21:I23"/>
+    <mergeCell ref="G21:G23"/>
+    <mergeCell ref="E21:E23"/>
+    <mergeCell ref="I37:I39"/>
+    <mergeCell ref="I24:I25"/>
+    <mergeCell ref="D27:D29"/>
+    <mergeCell ref="I34:I35"/>
+    <mergeCell ref="G34:G35"/>
+    <mergeCell ref="F34:F35"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="E27:E29"/>
+    <mergeCell ref="I27:I29"/>
+    <mergeCell ref="F27:F29"/>
+    <mergeCell ref="E11:E13"/>
+    <mergeCell ref="F11:F13"/>
+    <mergeCell ref="I11:I13"/>
+    <mergeCell ref="G11:G13"/>
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="H24:H25"/>
+    <mergeCell ref="I15:I17"/>
+    <mergeCell ref="D18:D20"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="B46:I46"/>
+    <mergeCell ref="G40:G42"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="G30:G31"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="D21:D23"/>
+    <mergeCell ref="F21:F23"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="H15:H17"/>
+    <mergeCell ref="A2:A43"/>
+    <mergeCell ref="A44:A47"/>
+    <mergeCell ref="B40:B42"/>
+    <mergeCell ref="C40:C42"/>
+    <mergeCell ref="H4:H6"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="H21:H23"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="G4:G6"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="H30:H31"/>
+    <mergeCell ref="E15:E17"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="H9:H10"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="E4:E6"/>
     <mergeCell ref="F4:F6"/>
@@ -2100,70 +2164,6 @@
     <mergeCell ref="E9:E10"/>
     <mergeCell ref="G15:G17"/>
     <mergeCell ref="F15:F17"/>
-    <mergeCell ref="A2:A43"/>
-    <mergeCell ref="A44:A47"/>
-    <mergeCell ref="B40:B42"/>
-    <mergeCell ref="C40:C42"/>
-    <mergeCell ref="H4:H6"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="H21:H23"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="G4:G6"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="H30:H31"/>
-    <mergeCell ref="E15:E17"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="B46:I46"/>
-    <mergeCell ref="G40:G42"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="G30:G31"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="B27:B29"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="F30:F31"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="D21:D23"/>
-    <mergeCell ref="F21:F23"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="H15:H17"/>
-    <mergeCell ref="D18:D20"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="E11:E13"/>
-    <mergeCell ref="F11:F13"/>
-    <mergeCell ref="I11:I13"/>
-    <mergeCell ref="G11:G13"/>
-    <mergeCell ref="G24:G25"/>
-    <mergeCell ref="H24:H25"/>
-    <mergeCell ref="I15:I17"/>
-    <mergeCell ref="D27:D29"/>
-    <mergeCell ref="I34:I35"/>
-    <mergeCell ref="G34:G35"/>
-    <mergeCell ref="F34:F35"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="E27:E29"/>
-    <mergeCell ref="I27:I29"/>
-    <mergeCell ref="F27:F29"/>
-    <mergeCell ref="I40:I42"/>
-    <mergeCell ref="H18:H20"/>
-    <mergeCell ref="G18:G20"/>
-    <mergeCell ref="F18:F20"/>
-    <mergeCell ref="E18:E20"/>
-    <mergeCell ref="H36:H39"/>
-    <mergeCell ref="I30:I31"/>
-    <mergeCell ref="I21:I23"/>
-    <mergeCell ref="G21:G23"/>
-    <mergeCell ref="E21:E23"/>
-    <mergeCell ref="I37:I39"/>
-    <mergeCell ref="I24:I25"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>